<commit_message>
DA 20 | Day 8
</commit_message>
<xml_diff>
--- a/Batch/19/Day_8.xlsx
+++ b/Batch/19/Day_8.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29204"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\excel\Batch\19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CECBDB-FED9-4FC5-B8B3-F9544A2D66AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF51BC7-8C98-41D8-8D08-CB1823E5DD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="741" activeTab="6" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
   </bookViews>
@@ -15701,7 +15701,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -15774,7 +15774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -15797,11 +15797,10 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -15841,8 +15840,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>169601</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
@@ -15861,7 +15860,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Ink 4">
@@ -15906,8 +15905,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>173119</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="6" name="Ink 5">
@@ -15926,7 +15925,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="6" name="Ink 5">
@@ -15971,8 +15970,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>191</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -15991,7 +15990,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -16036,8 +16035,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>8918</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="17" name="Ink 16">
@@ -16056,7 +16055,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="17" name="Ink 16">
@@ -16101,8 +16100,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="19" name="Ink 18">
@@ -16121,7 +16120,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="19" name="Ink 18">
@@ -16166,8 +16165,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>8877</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="20" name="Ink 19">
@@ -16186,7 +16185,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="20" name="Ink 19">
@@ -16231,8 +16230,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>171998</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="21" name="Ink 20">
@@ -16251,7 +16250,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="21" name="Ink 20">
@@ -16296,8 +16295,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>10759</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="25" name="Ink 24">
@@ -16316,7 +16315,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="25" name="Ink 24">
@@ -16361,8 +16360,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>9761</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="26" name="Ink 25">
@@ -16381,7 +16380,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="26" name="Ink 25">
@@ -16426,8 +16425,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>35877</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="30" name="Ink 29">
@@ -16446,7 +16445,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="30" name="Ink 29">
@@ -16491,8 +16490,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>87356</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="42" name="Ink 41">
@@ -16511,7 +16510,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="42" name="Ink 41">
@@ -16556,8 +16555,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>103158</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="47" name="Ink 46">
@@ -16576,7 +16575,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="47" name="Ink 46">
@@ -16621,8 +16620,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>58196</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="58" name="Ink 57">
@@ -16641,7 +16640,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="58" name="Ink 57">
@@ -16686,8 +16685,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>154555</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="65" name="Ink 64">
@@ -16706,7 +16705,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="65" name="Ink 64">
@@ -16751,8 +16750,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="73" name="Ink 72">
@@ -16771,7 +16770,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="73" name="Ink 72">
@@ -16816,8 +16815,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>45874</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Ink 77">
@@ -16836,7 +16835,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Ink 77">
@@ -16881,8 +16880,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>156</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="87" name="Ink 86">
@@ -16901,7 +16900,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="87" name="Ink 86">
@@ -16946,8 +16945,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>75340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="95" name="Ink 94">
@@ -16966,7 +16965,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="95" name="Ink 94">
@@ -17011,8 +17010,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>76671</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="108" name="Ink 107">
@@ -17031,7 +17030,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="108" name="Ink 107">
@@ -17076,8 +17075,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>172857</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="114" name="Ink 113">
@@ -17096,7 +17095,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="114" name="Ink 113">
@@ -17141,8 +17140,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>58951</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="125" name="Ink 124">
@@ -17161,7 +17160,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="125" name="Ink 124">
@@ -17206,8 +17205,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>36713</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="128" name="Ink 127">
@@ -17226,7 +17225,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="128" name="Ink 127">
@@ -17271,8 +17270,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>87783</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="129" name="Ink 128">
@@ -17291,7 +17290,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="129" name="Ink 128">
@@ -17336,8 +17335,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>49560</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="153" name="Ink 152">
@@ -17356,7 +17355,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="153" name="Ink 152">
@@ -17401,8 +17400,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>124307</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="154" name="Ink 153">
@@ -17421,7 +17420,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="154" name="Ink 153">
@@ -17466,8 +17465,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>11658</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="171" name="Ink 170">
@@ -17486,7 +17485,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="171" name="Ink 170">
@@ -17531,8 +17530,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>160189</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="176" name="Ink 175">
@@ -17551,7 +17550,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="176" name="Ink 175">
@@ -17596,8 +17595,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>172871</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="179" name="Ink 178">
@@ -17616,7 +17615,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="179" name="Ink 178">
@@ -17661,8 +17660,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>11801</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId57">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="208" name="Ink 207">
@@ -17681,7 +17680,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="208" name="Ink 207">
@@ -17726,8 +17725,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>160909</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId59">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="209" name="Ink 208">
@@ -17746,7 +17745,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="209" name="Ink 208">
@@ -17791,8 +17790,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>7237</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="215" name="Ink 214">
@@ -17811,7 +17810,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="215" name="Ink 214">
@@ -17856,8 +17855,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>151093</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId63">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="221" name="Ink 220">
@@ -17876,7 +17875,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="221" name="Ink 220">
@@ -17921,8 +17920,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>58818</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId65">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="222" name="Ink 221">
@@ -17941,7 +17940,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="222" name="Ink 221">
@@ -17986,8 +17985,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>171809</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId67">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="233" name="Ink 232">
@@ -18006,7 +18005,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="233" name="Ink 232">
@@ -18051,8 +18050,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>159733</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId69">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="234" name="Ink 233">
@@ -18071,7 +18070,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="234" name="Ink 233">
@@ -18116,8 +18115,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>85458</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId71">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="238" name="Ink 237">
@@ -18136,7 +18135,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="238" name="Ink 237">
@@ -18181,8 +18180,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>858</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId73">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="256" name="Ink 255">
@@ -18201,7 +18200,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="256" name="Ink 255">
@@ -18246,8 +18245,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>17058</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId75">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="257" name="Ink 256">
@@ -18266,7 +18265,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="257" name="Ink 256">
@@ -18311,8 +18310,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>21100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId77">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="259" name="Ink 258">
@@ -18331,7 +18330,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="259" name="Ink 258">
@@ -18376,8 +18375,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>68192</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId79">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="263" name="Ink 262">
@@ -18396,7 +18395,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="263" name="Ink 262">
@@ -18441,8 +18440,8 @@
       <xdr:row>43</xdr:row>
       <xdr:rowOff>58045</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId81">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="270" name="Ink 269">
@@ -18461,7 +18460,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="270" name="Ink 269">
@@ -18506,8 +18505,8 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>112567</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId83">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="273" name="Ink 272">
@@ -18526,7 +18525,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="273" name="Ink 272">
@@ -18571,8 +18570,8 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>115169</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId85">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="285" name="Ink 284">
@@ -18591,7 +18590,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="285" name="Ink 284">
@@ -18636,8 +18635,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>96055</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId87">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="286" name="Ink 285">
@@ -18656,7 +18655,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="286" name="Ink 285">
@@ -18701,8 +18700,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>160937</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId89">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="287" name="Ink 286">
@@ -18721,7 +18720,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="287" name="Ink 286">
@@ -18766,8 +18765,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>35894</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId91">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="299" name="Ink 298">
@@ -18786,7 +18785,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="299" name="Ink 298">
@@ -18831,8 +18830,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>7732</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId93">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="300" name="Ink 299">
@@ -18851,7 +18850,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="300" name="Ink 299">
@@ -18896,8 +18895,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>150210</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId95">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="301" name="Ink 300">
@@ -18916,7 +18915,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="301" name="Ink 300">
@@ -18961,8 +18960,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>74298</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId97">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="311" name="Ink 310">
@@ -18981,7 +18980,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="311" name="Ink 310">
@@ -19026,8 +19025,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>17500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId99">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="312" name="Ink 311">
@@ -19046,7 +19045,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="312" name="Ink 311">
@@ -19091,8 +19090,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>131490</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId101">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="324" name="Ink 323">
@@ -19111,7 +19110,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="324" name="Ink 323">
@@ -19156,8 +19155,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>173332</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId103">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="334" name="Ink 333">
@@ -19176,7 +19175,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="334" name="Ink 333">
@@ -19265,8 +19264,8 @@
       <xdr:row>56</xdr:row>
       <xdr:rowOff>96551</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId106">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="345" name="Ink 344">
@@ -19285,7 +19284,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="345" name="Ink 344">
@@ -19374,8 +19373,8 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>20883</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId109">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="355" name="Ink 354">
@@ -19394,7 +19393,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="355" name="Ink 354">
@@ -19439,8 +19438,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId111">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="356" name="Ink 355">
@@ -19459,7 +19458,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="356" name="Ink 355">
@@ -19504,8 +19503,8 @@
       <xdr:row>63</xdr:row>
       <xdr:rowOff>17936</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId113">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="357" name="Ink 356">
@@ -19524,7 +19523,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="357" name="Ink 356">
@@ -19569,8 +19568,8 @@
       <xdr:row>61</xdr:row>
       <xdr:rowOff>160841</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId115">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="358" name="Ink 357">
@@ -19589,7 +19588,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="358" name="Ink 357">
@@ -19634,8 +19633,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>170527</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId117">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="359" name="Ink 358">
@@ -19654,7 +19653,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="359" name="Ink 358">
@@ -19699,8 +19698,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>124889</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId119">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="364" name="Ink 363">
@@ -19719,7 +19718,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="364" name="Ink 363">
@@ -19764,8 +19763,8 @@
       <xdr:row>61</xdr:row>
       <xdr:rowOff>170643</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId121">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="367" name="Ink 366">
@@ -19784,7 +19783,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="367" name="Ink 366">
@@ -19829,8 +19828,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>7169</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId123">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="368" name="Ink 367">
@@ -19849,7 +19848,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="368" name="Ink 367">
@@ -19894,8 +19893,8 @@
       <xdr:row>63</xdr:row>
       <xdr:rowOff>19736</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId125">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="369" name="Ink 368">
@@ -19914,7 +19913,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="369" name="Ink 368">
@@ -19959,8 +19958,8 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>45397</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId127">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="378" name="Ink 377">
@@ -19979,7 +19978,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="378" name="Ink 377">
@@ -20024,8 +20023,8 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>77797</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId129">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="386" name="Ink 385">
@@ -20044,7 +20043,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="386" name="Ink 385">
@@ -20089,8 +20088,8 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>86403</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId131">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="396" name="Ink 395">
@@ -20109,7 +20108,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="396" name="Ink 395">
@@ -20154,8 +20153,8 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>55083</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId133">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="400" name="Ink 399">
@@ -20174,7 +20173,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="400" name="Ink 399">
@@ -20219,8 +20218,8 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>59220</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId135">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="404" name="Ink 403">
@@ -20239,7 +20238,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="404" name="Ink 403">
@@ -20284,8 +20283,8 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>66862</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId137">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="414" name="Ink 413">
@@ -20304,7 +20303,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="414" name="Ink 413">
@@ -20349,8 +20348,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>133035</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId139">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="431" name="Ink 430">
@@ -20369,7 +20368,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="431" name="Ink 430">
@@ -20414,8 +20413,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>163995</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId141">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="432" name="Ink 431">
@@ -20434,7 +20433,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="432" name="Ink 431">
@@ -20479,8 +20478,8 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>133409</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId143">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="438" name="Ink 437">
@@ -20499,7 +20498,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="438" name="Ink 437">
@@ -20544,8 +20543,8 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>93915</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId145">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="442" name="Ink 441">
@@ -20564,7 +20563,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="442" name="Ink 441">
@@ -20609,8 +20608,8 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>106822</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId147">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="446" name="Ink 445">
@@ -20629,7 +20628,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="446" name="Ink 445">
@@ -20674,8 +20673,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>87638</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId149">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="469" name="Ink 468">
@@ -20694,7 +20693,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="469" name="Ink 468">
@@ -20739,8 +20738,8 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>142290</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId151">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="479" name="Ink 478">
@@ -20759,7 +20758,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="479" name="Ink 478">
@@ -20804,8 +20803,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>27044</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId153">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="480" name="Ink 479">
@@ -20824,7 +20823,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="480" name="Ink 479">
@@ -20869,8 +20868,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>19238</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId155">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="482" name="Ink 481">
@@ -20889,7 +20888,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="482" name="Ink 481">
@@ -20934,8 +20933,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>28238</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId157">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="483" name="Ink 482">
@@ -20954,7 +20953,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="483" name="Ink 482">
@@ -20999,8 +20998,8 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>7420</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId159">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="484" name="Ink 483">
@@ -21019,7 +21018,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="484" name="Ink 483">
@@ -21064,8 +21063,8 @@
       <xdr:row>80</xdr:row>
       <xdr:rowOff>67669</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId161">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="489" name="Ink 488">
@@ -21084,7 +21083,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="489" name="Ink 488">
@@ -21129,8 +21128,8 @@
       <xdr:row>80</xdr:row>
       <xdr:rowOff>153</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId163">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="490" name="Ink 489">
@@ -21149,7 +21148,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="490" name="Ink 489">
@@ -21194,8 +21193,8 @@
       <xdr:row>84</xdr:row>
       <xdr:rowOff>105795</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId165">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="531" name="Ink 530">
@@ -21214,7 +21213,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="531" name="Ink 530">
@@ -21259,8 +21258,8 @@
       <xdr:row>85</xdr:row>
       <xdr:rowOff>133563</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId167">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="549" name="Ink 548">
@@ -21279,7 +21278,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="549" name="Ink 548">
@@ -21324,8 +21323,8 @@
       <xdr:row>86</xdr:row>
       <xdr:rowOff>11407</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId169">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="565" name="Ink 564">
@@ -21344,7 +21343,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="565" name="Ink 564">
@@ -21389,8 +21388,8 @@
       <xdr:row>85</xdr:row>
       <xdr:rowOff>163803</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId171">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="581" name="Ink 580">
@@ -21409,7 +21408,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="581" name="Ink 580">
@@ -21454,8 +21453,8 @@
       <xdr:row>84</xdr:row>
       <xdr:rowOff>125317</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId173">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="591" name="Ink 590">
@@ -21474,7 +21473,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="591" name="Ink 590">
@@ -21519,8 +21518,8 @@
       <xdr:row>87</xdr:row>
       <xdr:rowOff>164096</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId175">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="594" name="Ink 593">
@@ -21539,7 +21538,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="594" name="Ink 593">
@@ -21584,8 +21583,8 @@
       <xdr:row>87</xdr:row>
       <xdr:rowOff>123334</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId177">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="595" name="Ink 594">
@@ -21604,7 +21603,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="595" name="Ink 594">
@@ -21649,8 +21648,8 @@
       <xdr:row>88</xdr:row>
       <xdr:rowOff>56340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId179">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="596" name="Ink 595">
@@ -21669,7 +21668,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="596" name="Ink 595">
@@ -21714,8 +21713,8 @@
       <xdr:row>87</xdr:row>
       <xdr:rowOff>8658</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId181">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="597" name="Ink 596">
@@ -21734,7 +21733,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="597" name="Ink 596">
@@ -21779,8 +21778,8 @@
       <xdr:row>89</xdr:row>
       <xdr:rowOff>173666</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId183">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="598" name="Ink 597">
@@ -21799,7 +21798,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="598" name="Ink 597">
@@ -21844,8 +21843,8 @@
       <xdr:row>90</xdr:row>
       <xdr:rowOff>20992</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId185">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="601" name="Ink 600">
@@ -21864,7 +21863,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="601" name="Ink 600">
@@ -21909,8 +21908,8 @@
       <xdr:row>89</xdr:row>
       <xdr:rowOff>173748</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId187">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="604" name="Ink 603">
@@ -21929,7 +21928,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="604" name="Ink 603">
@@ -21974,8 +21973,8 @@
       <xdr:row>93</xdr:row>
       <xdr:rowOff>94855</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId189">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="612" name="Ink 611">
@@ -21994,7 +21993,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="612" name="Ink 611">
@@ -22088,8 +22087,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>675</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -22108,7 +22107,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -22153,8 +22152,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>928</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -22173,7 +22172,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -22218,8 +22217,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>169996</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="20" name="Ink 19">
@@ -22238,7 +22237,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="20" name="Ink 19">
@@ -22283,8 +22282,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>180120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="29" name="Ink 28">
@@ -22303,7 +22302,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="29" name="Ink 28">
@@ -22348,8 +22347,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>170760</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="33" name="Ink 32">
@@ -22368,7 +22367,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="33" name="Ink 32">
@@ -22413,8 +22412,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>16700</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="51" name="Ink 50">
@@ -22433,7 +22432,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="51" name="Ink 50">
@@ -22478,8 +22477,8 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>21064</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="52" name="Ink 51">
@@ -22498,7 +22497,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="52" name="Ink 51">
@@ -22589,7 +22588,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2020.31">60 17 1072,'0'0'14965,"-7"-3"-13954,6 3-1035,-25-7 822,20 2-281,21 4-320,266 1 329,-186 0-3600,0 0-4366</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1599.47">248 65 13126,'0'0'7491,"0"-10"-7122,11 188-442,-1 4 79,-10-181-2,0 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1-1 1,0 0 0,1 1-1,-1-1 1,1 0-1,-1 1 1,0-1 0,1 0-1,-1 0 1,0 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,-25-1 137,24 1-118,-153 0 177,142-3-1213,11-7-2824,2-1-1995</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-931.58">957 159 11381,'0'0'6723,"0"-11"-5954,0-33-228,0 33 433,-28 11-160,25 2-813,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 1 1,0-1-1,1 1 1,-1-1-1,1 1 1,-1 0 0,1 0-1,0 0 1,0 0-1,-2 4 1,-25 57 65,25-52-32,0 1-1,1 0 0,1 0 1,0 0-1,0 0 1,1 1-1,1-1 1,1 0-1,2 18 1,-2-26-24,0 0 0,1 1 0,-1-1 0,1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 1,1-1-1,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,0-1 0,0 0 0,0 1 0,0-2 0,0 1 0,9 1 0,-5 0 2,0-1 0,0 0 0,1-1 0,-1 0-1,1-1 1,-1 0 0,1 0 0,-1-1 0,1 0-1,-1-1 1,0 0 0,1 0 0,-1-1 0,0 0-1,-1-1 1,1 0 0,-1 0 0,1-1 0,-1 0-1,0 0 1,-1-1 0,0 0 0,0 0 0,0-1 0,0 0-1,-1 0 1,0-1 0,-1 1 0,0-1 0,0-1-1,-1 1 1,1-1 0,-2 1 0,1-1 0,-2 0-1,1 0 1,-1-1 0,0 1 0,0-13 0,-1 12-12,-1-1-1,0 1 1,-1-1 0,0 1 0,0-1 0,-1 1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,-8-16 0,8 19-1,-1 1 1,0 0-1,0 0 1,-1 0-1,0 0 1,1 1-1,-2 0 0,1 0 1,-1 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0 0 0,-1 0 1,-8-1-1,5 1-429,0 1-1,-1-1 0,1 2 1,-1 0-1,1 0 1,-1 1-1,-20 3 0,29-3 247,0 1 1,0-1-1,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,2 0 0,-1 0 1,0 0-1,0 0 0,1 0 0,0 0 0,0 0 0,0 4 0,0 10-6921</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14502.86">272 689 10101,'0'0'9991,"-13"-5"-9663,3 1-281,0 1-1,-1 0 1,1 0 0,-1 1-1,-19-2 1,25 4-28,1 0-1,-1 0 1,0 1 0,1-1-1,-1 1 1,1 0 0,-1 1-1,1-1 1,-1 1 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1-1,0 0 1,1-1 0,-1 2-1,1-1 1,-6 7 0,3-2 15,-1 1 1,2 0-1,-1 1 1,2-1-1,-1 1 1,1 0-1,0 0 1,1 0-1,1 1 1,-1-1 0,2 1-1,-1-1 1,1 1-1,1 0 1,0-1-1,1 1 1,3 19-1,-3-27-46,0 1 1,1 0-1,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 0 1,0-1-1,0 1 0,-1-1 0,1 1 0,0-1 0,0-1 0,1 1 0,-1 0 1,0-1-1,0 0 0,0 0 0,8-1 0,-11 0 34,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1-1-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,0 0 0,-1-1 1,1 1-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 0,0 0 1,-2 0-1,-11-1 90,0 0 0,0 1 0,-17 0 0,27 1-111,1 0 0,0 0 1,0 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0 0 1,0-1-1,0 1 0,1 0 1,-1 0-1,1 0 0,-1 1 1,-1 2-1,4-5-94,-1 0 0,1 1 0,0-1 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1-1,0-1 1,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 1 1,16 0-5466,-15-1 5368,10 0-5691</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14502.85">272 689 10101,'0'0'9991,"-13"-5"-9663,3 1-281,0 1-1,-1 0 1,1 0 0,-1 1-1,-19-2 1,25 4-28,1 0-1,-1 0 1,0 1 0,1-1-1,-1 1 1,1 0 0,-1 1-1,1-1 1,-1 1 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1-1,0 0 1,1-1 0,-1 2-1,1-1 1,-6 7 0,3-2 15,-1 1 1,2 0-1,-1 1 1,2-1-1,-1 1 1,1 0-1,0 0 1,1 0-1,1 1 1,-1-1 0,2 1-1,-1-1 1,1 1-1,1 0 1,0-1-1,1 1 1,3 19-1,-3-27-46,0 1 1,1 0-1,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 0 1,0-1-1,0 1 0,-1-1 0,1 1 0,0-1 0,0-1 0,1 1 0,-1 0 1,0-1-1,0 0 0,0 0 0,8-1 0,-11 0 34,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1-1-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,0 0 0,-1-1 1,1 1-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 0,0 0 1,-2 0-1,-11-1 90,0 0 0,0 1 0,-17 0 0,27 1-111,1 0 0,0 0 1,0 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0 0 1,0-1-1,0 1 0,1 0 1,-1 0-1,1 0 0,-1 1 1,-1 2-1,4-5-94,-1 0 0,1 1 0,0-1 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1-1,0-1 1,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 1 1,16 0-5466,-15-1 5368,10 0-5691</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15340.65">801 699 7443,'0'0'13121,"-17"-10"-11312,172 16-1516,-156 34-615,-6-12 540,0 0 0,-2 0 0,-15 30 0,-3 10 139,14-35-167,9-26-123,1 0 0,0 0 0,0 1 0,1 0 0,0-1 0,0 1 0,-1 13 0,3-20 96,1-22-4053,2 7-2265,4-2-6213</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16436.04">1630 880 12726,'0'0'8804,"1"-1"-8725,-1 0 0,0-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,0 0 0,-1 0 0,1-1 1,0 1-1,-1 0 0,1 0 0,-2-3 1,-4 6-56,1 0 1,0 0-1,-1 0 0,1 1 1,0-1-1,1 1 1,-1 1-1,0-1 1,1 0-1,0 1 1,0 0-1,0 0 1,0 0-1,1 1 0,-4 5 1,4-7-17,0 2-1,0-1 1,0 0 0,1 0 0,0 1-1,0-1 1,0 1 0,0 0 0,1 0 0,0-1-1,0 1 1,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,2 7 0,-2-11-9,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0-1,0 0 1,1 1 0,-1-1 0,0 0 0,3-1 0,37 1 191,-29-1-126,-8 1-58,8 1 9,-1-2 0,0 1 0,1-1 0,-1-1-1,19-4 1,-28 5-19,1 0-1,-1 0 0,1 0 1,-1-1-1,1 1 0,-1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 1,0-1-1,0 1 0,0-1 1,0 1-1,-1-1 0,1 0 1,-1 1-1,0-1 0,1 0 1,-2-5-1,1 4-10,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,-3-4 0,-1 0 31,-1 1-1,1 0 1,-1 0 0,-15-8-1,20 13-9,-1-1-8,0 0 1,1-1-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,0-1 1,-1 1-1,1 0 1,1-1-1,-1 1 1,0 0-1,1-1 1,0 1-1,0-1 1,0 1-1,0 0 0,0-1 1,2-5-1,-2-11 47,0 18-66,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,1 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,1 0-1,1-1 0,0 1-16,-1 1-1,1-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 1 0,1 0 1,-1 0-1,3 0 0,-3 0 36,0-1-1,1 1 0,-1 0 0,0 1 1,0-1-1,0 0 0,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0 1 0,0-1 1,0 0-1,-1 1 0,1 0 1,3 3-1,-4-2-5,0 1 0,0-1-1,0 1 1,-1 0 0,1-1 0,-1 1 0,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,-1 7-1,2-4 5,-1 0-1,-1 0 0,1-1 0,-1 1 1,0 0-1,-1 0 0,1-1 1,-5 12-1,3-14 0,1-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,-1-1 1,1 1-1,-1-1 0,0 0 1,0 0-1,-6 2 0,-3 2-188,-15 5-1529,9-6-3040,4-4-3685</inkml:trace>
 </inkml:ink>
@@ -22624,7 +22623,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="956.05">2062 159 14711,'0'0'4354</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1998.14">2099 337 14295,'0'0'9012,"-4"7"-8708,0 0-206,0-2 5,1 0 0,0 1-1,0-1 1,1 1 0,-1-1 0,1 1-1,0 0 1,1 0 0,-2 8 0,34-23-207,7-13 242,-29 16-168,0 1 1,0-1-1,1 2 0,0-1 0,17-4 1,-21 8 26,-5 28-288,-8 71 635,37-99-450,-25 0 123,1-1 0,-1 1 0,0-1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 1,-1-1-1,0 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,-1-1 0,1-7 0,-2 12-54,-1 10-137,0-6 145,0-1 0,0 1 0,1-1 0,-1 0 1,1 1-1,0-1 0,0 1 0,0-1 0,0 1 1,1 3-1,5-8 52,-1 0 1,1-1-1,0 1 0,0-1 1,-1-1-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 0 0,-1 0 1,-1 0-1,6-8 0,-9 13-17,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,20 0 82,21-10 37,-24-2-123,0-1-1,-1-1 1,-1 0-1,0-1 1,-1-1-1,0 0 1,-2-1-1,0 0 1,0-1 0,-2-1-1,0 0 1,-2 0-1,10-30 1,-33 78-100,0 1 1,2 0 0,2 1 0,-9 34 0,19-56 113,-1 2-18,1-1 1,0 1 0,1-1-1,1 20 1,-1-28-4,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 1,0 1-1,1-1 1,-1 1-1,1-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,4-1-1,6 2 8,1-1 0,-1-1 0,1 0 0,0-1 0,-1 0 0,1-1 0,0 0 0,-1-1 0,0 0 0,0-1 0,0-1 0,0 0 0,-1 0 0,0-1 0,0 0 0,14-11 0,-24 16-11,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 0 0,-1 1 1,0-1-1,1 1 0,-1-1 0,0 0 0,-1-2 1,1 3 0,-1 0 0,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 1 0,0-1 0,0 0 1,0 1-1,-1-1 0,1 1 0,0 0 1,0-1-1,-1 1 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-3 0 0,-1 0 9,0 1-1,1-1 1,-1 1 0,0 0-1,0 0 1,1 0 0,-1 1-1,0-1 1,1 1 0,0 1-1,-1-1 1,1 0 0,0 1-1,0 0 1,0 0 0,1 0-1,-1 0 1,1 1 0,0 0-1,-5 6 1,3-3-13,1 0 1,0 1-1,1-1 1,0 1 0,0-1-1,0 1 1,1 0-1,1 0 1,-1 0-1,1 0 1,0 14-1,1-21-79,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1-1 0,2 1 0,9-1-8564</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2139.19">2517 151 15367,'0'0'6291,"112"-44"-9220,-42 44-2322</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2542.18">3429 219 16680,'0'0'5245,"0"-12"-4410,-3-37-190,3 48-626,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,0 4-28,0 0-1,0 0 1,0 0-1,1 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,1 0-1,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-1,5 10 1,3 7 23,1-1 0,22 37 0,-30-57 6,1 2-24,0 1 1,-1-1-1,1 1 0,-1 0 1,0 0-1,2 9 0,-4-14 1,0 1 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 1,0-1-1,0 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1 0 0,-1-1 1,1 0-1,-1 1 0,0 0 0,-23 4 121,2-4 448,10 0-1985,1-1-6284</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2542.17">3429 219 16680,'0'0'5245,"0"-12"-4410,-3-37-190,3 48-626,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,0 4-28,0 0-1,0 0 1,0 0-1,1 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,1 0-1,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-1,5 10 1,3 7 23,1-1 0,22 37 0,-30-57 6,1 2-24,0 1 1,-1-1-1,1 1 0,-1 0 1,0 0-1,2 9 0,-4-14 1,0 1 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 1,0-1-1,0 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1 0 0,-1-1 1,1 0-1,-1 1 0,0 0 0,-23 4 121,2-4 448,10 0-1985,1-1-6284</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3832.37">3612 265 6259,'0'0'9124,"6"-12"-6173,21-35-753,-22 30 1733,-13 17-3299,-10 11-900,11-4 364,-1 0 0,1 0 1,0 1-1,0 0 0,1 1 0,-7 12 0,10-17-122,1 1 1,-1 0-1,1-1 1,1 1 0,-1 0-1,1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1 1-1,0-1 1,0 0 0,2 9-1,-1-13-53,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,2 0 0,44 3-2390,-39-3 1558,-2 0 104,0 0 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,0 0 0,9-7 0,-12 7 615,1 0-1,-1 0 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 0-1,4-7 1,-4 6 1229,0 0 0,0-1 0,-1 1 0,1-1 1,-1 1-1,-1-1 0,1-10 0,-1 16-794,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 1 0,-1-1-1,1 1 1,-1 0 0,1-1 0,-2 1 0,-15 4 1696,-14 22-1790,29-23-139,0 0 0,-1 0 0,2 1 0,-1-1 0,0 1 0,1-1 0,0 1 0,-1 0 0,1-1 0,1 1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,1 5 0,-1-7-45,0 0-1,1 1 1,-1-1-1,1 0 1,-1 0 0,1 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0-1-1,0 1 1,0-1-1,3 1 1,52 5-1076,-47-6-404,1-1 1,-1 1-1,1-2 1,-1 0-1,15-4 0,-17 4 321,0-2-1,0 1 0,-1-1 0,1 0 1,-1 0-1,0-1 0,8-6 0,23-32-752,-36 40 2308,22-35 4977,-16 11 7954,-17 52-12201,9-24-1081,-4 10 121,1-1 0,1 1 0,0 0-1,-1 18 1,6-28-114,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,6-2 0,-4 0-13,1 0 0,-1 0 0,0-1 0,1 1 0,-1-1 0,7-5 0,6-4 267,-13 72 1861,-4-58-2212,1-1 0,-1 1-1,1 0 1,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1-1,0-1 1,0 1 0,4-1 0,45 5-3786,-42-4 2764,1-1 0,-1 0 0,0 0 1,1-1-1,-1-1 0,0 1 0,10-4 0,-17 4 1085,1 0-1,-1 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 1,0-1-1,-1 0 0,1 0 1,0 1-1,2-5 1,-3 2 735,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 1 0,0-7 0,0 9-627,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,-1 0 0,0 0-1,1 1 1,-1-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 1 0,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,-1 1-1,-1 0 33,1-1-1,-1 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 1 1,0 0-1,-3 3 0,4-4-127,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,0 0 1,-1-1-1,1 1 1,0 0 0,-1-1-1,1 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,1 1-1,-1 0 1,2 0-22,-1 0 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,3-1 0,4-1-128,1 0-1,-2 0 1,1-1-1,14-7 1,-7 0-57,-1-1 1,0 0 0,0-1-1,-1-1 1,-1 0 0,0-1-1,-1 0 1,-1-1 0,0 0-1,14-29 1,-18 31 372,0-1 1,-1 0-1,0 0 1,-1-1-1,-1 1 0,0-1 1,-1 0-1,0-15 0,-19 60 496,7-8-615,1 1-1,1 1 1,1-1 0,2 1 0,0 0 0,1 0 0,1 1 0,2-1 0,1 35-1,0-58-45,0 0-1,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 0,-1 1 1,1 0-1,0-1 1,-1 1-1,1-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,1 1 1,26-4-67,26-26-178,-51 26 189,98-61-199,-120 110 1489,15-42-1333,0 0-1,0 0 0,-1 0 0,1 0 1,-1-1-1,0 0 0,0 0 0,-1 0 0,1 0 1,-1-1-1,1 0 0,-1 0 0,0-1 1,0 1-1,1-1 0,-1 0 0,0-1 1,-12 0-1,-29 1-5363</inkml:trace>
 </inkml:ink>
 </file>
@@ -22725,7 +22724,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">170 3 9108,'0'0'8924,"0"-3"-7651,-1 7-1062,-2 9-73,-1-1 0,-1 0 0,0 0 1,-1 0-1,0-1 0,-1 0 1,0 0-1,-11 12 0,-16 27 106,16-19-169,-38 71 232,83-151-605,62-86 1,-43 69 177,-27 47 121,-18 19-10,-1 0 1,1 0-1,-1 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 1 0,1-1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,0 0 1,1 2 9,1 1 1,0 0-1,-1 0 0,0 0 1,0 0-1,0 0 0,1 8 1,6 18 314,-1 0 1,6 60 0,-2-8 219,-11-76 199,1 5-3588,-1-32-10479</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="294.76">135 203 8516,'0'0'10735,"4"-3"-10454,4 0-96,1-1 0,-1 1 0,1 0 0,0 1 0,0 0 1,0 1-1,0-1 0,14 1 0,18-3-1390,5-4-4608</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="764.72">815 76 9412,'0'0'8297,"-25"-12"-7315,18 13-939,0 0 0,0 0 0,0 1 0,0 0-1,1 0 1,-1 0 0,1 1 0,-1 0 0,1 0 0,0 1-1,0 0 1,1 0 0,-1 0 0,-6 7 0,-6 7 281,1 0-1,-26 35 1,40-49-304,0 0 0,0 0-1,1 0 1,0 1-1,-1-1 1,2 1 0,-1 0-1,0-1 1,1 1-1,0 0 1,0 0 0,0 0-1,1 0 1,0 0 0,-1 0-1,2 5 1,0-7-15,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,1 0 1,-1 0-1,0 1 0,1-1 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 1,-1-1-1,1 0 0,0 0 0,-1 1 1,4-2-1,4 2 31,-1-2 1,1 1-1,-1-1 1,1-1-1,-1 1 0,1-2 1,-1 1-1,0-1 1,0-1-1,13-6 0,-17 7-1052,-1 0-1,1 0 1,0-1-1,-1 1 1,0-1-1,7-8 1,-6 2-5793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1267.36">1263 74 10853,'0'0'9145,"-33"-17"-7530,24 17-1612,1 0 1,0 1-1,-1 0 1,1 0-1,0 0 1,0 1 0,0 0-1,0 1 1,0 0-1,1 0 1,-1 1 0,1 0-1,0 0 1,0 1-1,0 0 1,0 0-1,1 0 1,0 1 0,0 0-1,1 0 1,-1 0-1,1 1 1,1 0 0,-1 0-1,1 0 1,0 1-1,1-1 1,0 1-1,0 0 1,1 0 0,0 0-1,0 0 1,1 0-1,-1 13 1,2-17-17,-1 0 1,1 0-1,1 1 0,-1-1 1,1 0-1,0 0 1,-1 1-1,2-1 0,-1 0 1,0 0-1,1 0 0,0-1 1,4 8-1,-3-9-13,-1 1 0,1-1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1-1 0,0 1 0,5-1-1,4 2-1047,1-1-1,0-1 1,-1 0-1,1-1 1,0 0-1,-1-1 1,18-5-1,-5-4-4978</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1267.35">1263 74 10853,'0'0'9145,"-33"-17"-7530,24 17-1612,1 0 1,0 1-1,-1 0 1,1 0-1,0 0 1,0 1 0,0 0-1,0 1 1,0 0-1,1 0 1,-1 1 0,1 0-1,0 0 1,0 1-1,0 0 1,0 0-1,1 0 1,0 1 0,0 0-1,1 0 1,-1 0-1,1 1 1,1 0 0,-1 0-1,1 0 1,0 1-1,1-1 1,0 1-1,0 0 1,1 0 0,0 0-1,0 0 1,1 0-1,-1 13 1,2-17-17,-1 0 1,1 0-1,1 1 0,-1-1 1,1 0-1,0 0 1,-1 1-1,2-1 0,-1 0 1,0 0-1,1 0 0,0-1 1,4 8-1,-3-9-13,-1 1 0,1-1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1-1 0,0 1 0,5-1-1,4 2-1047,1-1-1,0-1 1,-1 0-1,1-1 1,0 0-1,-1-1 1,18-5-1,-5-4-4978</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -22824,7 +22823,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">47 146 6371,'0'0'11184,"7"-9"-10320,-7 24-665,-1 1 0,-1-1 0,0 0 0,-1 0 0,0 0 0,-2 0-1,1-1 1,-11 22 0,14-35-163,1-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 1 1,-1-1-1,1 0 0,-1 1 1,1-1-1,-1 0 1,1 0-1,-1 1 1,1-1-1,-2 0 1,-3-13 345,3-27-410,2 39 28,0-6 8,1 0 0,0 0 0,0 1 0,1-1 0,0 0 0,0 1 0,1-1 0,0 1 0,0 0 1,0 0-1,1 0 0,0 0 0,7-9 0,-7 11-27,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 1-1,1-1 0,-1 1 0,0 1 1,1-1-1,-1 1 0,1 0 0,7-1 1,-11 3 6,-1 0-1,0-1 1,0 1 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,-1 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0 2-1,3 45 41,-3-46-22,-1 15-61,1 6 703,1-24-638,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 0-1,1-1 1,0 1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 1 0,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1-1 0,9-7-63,1 0 1,0 1-1,0 0 0,1 0 1,0 1-1,0 1 1,0 0-1,0 1 1,1 0-1,0 0 1,0 1-1,21-2 0,-33 6 46,1 0 1,0 0-1,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,-1 3 0,3 29 28,-3-11 88,0-15-59,0-1 0,1 1 0,0-1-1,0 0 1,1 1 0,-1-1 0,3 7 0,-2-12-44,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,2-1 0,30-2 243,-25 1-226,0 0 0,1-1 0,-1-1 0,0 0 0,0 0 0,-1 0 0,12-8 1,-17 10-44,1-1 0,-1 1 0,0-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0-1 0,-1 1 1,0 0-1,1-1 0,-1 1 0,-1-1 1,1 0-1,0 0 0,-1 0 1,0 0-1,0 0 0,1-6 1,-2 9-4,-4 6-75,0-1 51,0 1 0,1-1 0,0 1 0,0 0 0,0 0 0,-3 8 0,5-12 32,1 0-21,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,0 0-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 1 1,-1-1 0,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,1 1 1,1-1-434,1 0 0,-1 0 1,1-1-1,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1-1 1,1 1-1,3-2 0,17-4-5420</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="156.31">687 107 5539,'0'0'13622,"4"-10"-14150,-1 12-609,8 11-992,0-3-2129,6 2-1553</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="612.66">951 186 6851,'0'0'8337,"-14"-3"-7176,1-1-926,0 1-1,-1 1 1,1 0 0,0 1 0,-25 0 0,35 1-215,-1 0 1,0 1-1,1-1 0,-1 1 1,1-1-1,-1 1 1,1 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 0,-1 0 1,2 0-1,-1 0 1,0 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,0 1-1,0 4 0,1-7-36,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,0 0 0,1 0 0,28 2 167,-23-4 8,0 0-130,0 0 0,0-1 0,0 0 0,0 0-1,0-1 1,-1 1 0,1-2 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1-1-1,1 0 1,-1 0 0,-1 0 0,5-7 0,10-13-74,-1-2 0,21-40 0,-35 61 29,27-64 179,-28 59 531,-22 45-260,13-21-401,0 0-1,1 0 1,1 0 0,0 1-1,1-1 1,0 1-1,1 0 1,0 0-1,1 0 1,2 20-1,-1-31-208,1-1 0,-1 0 1,0 0-1,1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 1,-1 0-1,1-1 0,0 1 0,0-1 0,2 3 0,0-2-622,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1-1-1,0 0 1,6 1-1,20 0-5579</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="816.36">1181 225 8612,'0'0'9828,"-11"-4"-10116,19 4-80,6 0 368,3-2 272,5 0-272,3 0-144,3 0-1537,-3 2-656,-8 0-2369,-2 0-608</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="816.35">1181 225 8612,'0'0'9828,"-11"-4"-10116,19 4-80,6 0 368,3-2 272,5 0-272,3 0-144,3 0-1537,-3 2-656,-8 0-2369,-2 0-608</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="999.97">1240 287 6675,'0'0'10757,"-25"14"-10757,29-10-544,14-4-33,3 0 369,11 0-560,3 0-1473,4-2-3890</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1307.07">1330 118 2977,'0'0'15885,"-6"-4"-14850,-7-6-952,7 5-486,22 21 179,10 7 156,-18-17 86,-1 0 0,1 1 0,-1 0 0,0 0 0,-1 1 0,11 15 0,-16-21-3,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,-1 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,-1-1 1,0 1-1,1-1 1,-1 0 0,0 1-1,0-1 1,0 0-1,0 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1-1,-5 3 1,-53 38 706,-9 6-959,32-10-6579</inkml:trace>
 </inkml:ink>
@@ -22918,7 +22917,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">12 11 1905,'0'0'5733,"-11"-10"1764,26 100-7249,-11-70-2358,0-10-4077,3-9 3215</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1084.14">239 52 5282,'0'0'6940,"0"-22"-2926,0-1-3314,1 22-718,-1 1 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 1 1,-1-1-1,1 0 1,-1 0-1,1 1 0,-1-1 1,0 0-1,1 1 1,-1-1-1,1 1 0,8 20-301,-5 22-247,-3-40 567,-1 1 0,0-1-1,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1 0,-4 3-1,-3 9-4,14-8-189,27-6-181,-14-2 481,20 1-6257</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1084.13">239 52 5282,'0'0'6940,"0"-22"-2926,0-1-3314,1 22-718,-1 1 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 1 1,-1-1-1,1 0 1,-1 0-1,1 1 0,-1-1 1,0 0-1,1 1 1,-1-1-1,1 1 0,8 20-301,-5 22-247,-3-40 567,-1 1 0,0-1-1,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1 0,-4 3-1,-3 9-4,14-8-189,27-6-181,-14-2 481,20 1-6257</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -22947,7 +22946,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 67 4898,'7'-4'14392,"5"-2"-16042,-13 22 1083,1-14 546,-1 0 0,1 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0-1 0,2 3 0,-2-4 14,-1 1 1,1-1-1,0 1 1,-1 0 0,1-1-1,-1 1 1,1 0-1,-1-1 1,0 1 0,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,1-1-1,-1 1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0-1,1-1 1,-1 2 0,0-1 69,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0-1 1,-1 1-1,1-1 0,-1 0 1,1 1-1,-1-1 1,1 0-1,-3 0 0,3 0-108</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="846.85">115 73 4322,'0'0'8070,"0"-13"-3420,0 15-4661,0 1 0,1 0 0,-1-1 0,1 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,1 1 0,-1-1 0,0 0-1,1 1 1,-1-1 0,3 3 0,-3-5-16,0 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0-1,-1-1 1,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0-1,0 0 1,1-1 0,9-7-74,-8 15-755,-5 25 941,-4-8 375,3-17-4831</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="846.84">115 73 4322,'0'0'8070,"0"-13"-3420,0 15-4661,0 1 0,1 0 0,-1-1 0,1 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,1 1 0,-1-1 0,0 0-1,1 1 1,-1-1 0,3 3 0,-3-5-16,0 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0-1,-1-1 1,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0-1,0 0 1,1-1 0,9-7-74,-8 15-755,-5 25 941,-4-8 375,3-17-4831</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1520.12">294 57 3009,'0'0'9229,"-21"15"-6943,20-13-2250,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 0,1 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,1 1 0,-1-1 1,1 0-1,-1 0 1,2 3-1,2 18-7069</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1731.31">296 57 5090,'0'0'6867,"23"-16"-6578,-16 13 79,-1 2-224,-2 0-64,0-1-16,0 2-64,-1 0-1217</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2741.47">427 34 2849,'-2'-3'13741,"-1"5"-13638,0 3-62,0 1 0,0-1 0,0 1 0,1 0 1,-1 0-1,1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 8 1,2-14-333,-1 0 239,1 1-1,0-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,0-1 0,0 1 1,0-1-1,1 0 0,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,-1 1 1,1-2-1,-10 2-5702</inkml:trace>
@@ -23171,7 +23170,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">34 393 9492,'0'0'4690,"86"-31"-4593,-65 31 31,-5 0-32,0 0-16,5 0 32,-1 0-96,5 0 16,-4 0-32,-1 5-144,-4 4-1185,-7-4-2193,-9 2-1856</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="215.98">1 529 7139,'0'0'5955,"115"-22"-5859,-78 15-16,0 0-16,-8 3-64,-5-3-720,-7 0-1937,-5 0-945</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="633.83">186 284 4066,'0'0'12675,"-12"-12"-11562,-34-33-292,34 34-42,23 34-797,-3-14 51,0-2 0,0 1 0,1-1 1,0 0-1,0-1 0,1 0 1,18 7-1,80 29 15,-78-31-72,11 2-41,-30-11-19,0 1 0,0 0-1,-1 1 1,1 0 0,-1 1-1,0 0 1,0 0 0,0 1 0,-1 1-1,13 10 1,-21-15 66,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-4 2 0,-8 6 25,0 0 0,0-1 1,-22 11-1,27-16-12,-64 31 158,45-23-52,0 1 0,2 1 0,-1 2 0,-37 28 1,61-42-274,1 0 1,-1 1-1,1-1 1,0 1 0,0-1-1,-1 1 1,1-1-1,0 1 1,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 2-1,25 0-13063</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="633.82">186 284 4066,'0'0'12675,"-12"-12"-11562,-34-33-292,34 34-42,23 34-797,-3-14 51,0-2 0,0 1 0,1-1 1,0 0-1,0-1 0,1 0 1,18 7-1,80 29 15,-78-31-72,11 2-41,-30-11-19,0 1 0,0 0-1,-1 1 1,1 0 0,-1 1-1,0 0 1,0 0 0,0 1 0,-1 1-1,13 10 1,-21-15 66,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-4 2 0,-8 6 25,0 0 0,0-1 1,-22 11-1,27-16-12,-64 31 158,45-23-52,0 1 0,2 1 0,-1 2 0,-37 28 1,61-42-274,1 0 1,-1 1-1,1-1 1,0 1 0,0-1-1,-1 1 1,1-1-1,0 1 1,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 2-1,25 0-13063</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1778.05">855 326 11013,'0'0'5149,"0"5"-4970,-2 8-5,0-1 1,0 1 0,-1-1-1,0 0 1,-10 22-1,-32 64 1188,45-98-1315,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,-1 1 0,1-1-1,0 1 1,0-1 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 1 1,0-1 0,-1 0 0,1 1-1,0-1 1,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,-1 0 0,1 1-1,-1-1 1,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,-3-20 592,5-31-593,2 40-93,0 1 0,1 0 0,0 0-1,1 1 1,0-1 0,1 1-1,0 0 1,0 0 0,1 1 0,0 0-1,0 0 1,1 0 0,0 1-1,0 0 1,1 1 0,0 0-1,0 0 1,0 1 0,1 0 0,0 1-1,17-6 1,-26 10 38,0 0 0,0 0 0,0-1 0,1 1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,1 0 0,-1 2 3,1 0 1,-1-1-1,0 1 0,1 0 0,-1 0 1,0 0-1,-1 0 0,1 0 1,0 3-1,1 12 25,-1-1 1,-2 29-1,0-24-45,1 13 109,0-34 165,0-39 176,1 33-466,0 0 0,0-1 0,1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,1 1 0,-1 0 0,1 0 0,5-3-1,-1 0-77,1 1-1,-1 0 0,1 1 1,-1 0-1,1 0 0,1 1 1,-1 1-1,0-1 0,18 0 1,-26 9 113,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-2 0 0,0 11 0,-1-6 99,-1 0 1,0 0 0,-1 0-1,0 0 1,-11 19 0,11-23-38,0 0 1,0 0 0,1 0 0,0 0-1,0 1 1,0-1 0,1 1 0,1 0 0,-1 0-1,1-1 1,1 1 0,-1 0 0,1 0-1,2 12 1,-1-19-46,0 1 0,0-1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,3-1 0,40 1 102,-33 0-70,-5 0-30,1-1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 0 0,0 0 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,5-8 0,-5 6-23,0-1 1,0 1 0,-1-1 0,0 0-1,0 0 1,-1 0 0,0 0-1,0 0 1,0-1 0,-1 0 0,-1 1-1,1-1 1,0-13 0,-2 20-36,-8 27-615,5-20 665,1-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,1 1-1,1-1 1,-1 0-1,1 0 1,1 12-1,0 0 0,-1-17-112,1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,2-1 0,33-8-5723,-19-4-876</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1948.36">1458 316 5234,'0'0'12086,"8"-23"-12086,-4 23-880,4 0-1073,-3 5 864,7 4-2801,-4 5-95</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2446.34">1680 396 5843,'0'0'10674,"-9"-5"-9935,5 2-711,0 0 1,0 0 0,-1 1-1,1 0 1,-1 0-1,0 0 1,0 1 0,0-1-1,0 1 1,0 0-1,0 1 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0 0 1,0 0 0,0 0-1,0 1 1,1-1-1,-1 1 1,0 0 0,1 1-1,-1-1 1,-6 6-1,7-6-18,1 0 0,-1 1 1,1-1-1,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 1,1 0-1,-1-1 0,0 1 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 5 0,2-8-3,0 0 0,-1-1-1,1 1 1,0 0-1,0-1 1,-1 1-1,1-1 1,0 0-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,1-1 1,28-6 405,-23 1-379,1 0 1,-1 0-1,0-1 1,-1 0-1,0 0 1,0 0-1,0-1 1,-1 0-1,0 0 1,4-10-1,6-17 50,14-43 1,-19 47-80,-17 93-818,-1-33 823,2 1-1,1 0 1,2 0-1,0 55 1,3-84-112,0 0 0,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 1,0-1-1,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,1 1 1,27 5-5103,2-5-2498</inkml:trace>
@@ -23182,7 +23181,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7213.69">3333 24 12870,'0'0'3025,"127"-23"-13333</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7626.99">4683 185 10645,'0'0'10245,"0"7"-10245,0 5 64,0 2-64,0 2 64,0-4-64,0 0 0,0-3-865,0-2-1376</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7780.05">4683 185 6995,'111'19'9989,"-111"-7"-9973,-12 6 64,7 1-80,1 2-1697,4-2-2785</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8047.97">5004 638 13862,'0'0'5443,"-29"37"-5315,13-25 112,-1 0-112,-3-3-128,3-2-1569,5-5-2160</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8047.96">5004 638 13862,'0'0'5443,"-29"37"-5315,13-25 112,-1 0-112,-3-3-128,3-2-1569,5-5-2160</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8961.94">5315 230 6659,'0'0'11408,"0"-8"-10197,0 6-1170,0-7 534,0 0 0,1 1 1,0-1-1,0 1 0,4-12 0,-4 19 407,0 6-442,-2 19-350,-9 34-325,-13-2 230,17-45-73,1 0 0,1 0 0,-1 1 1,2-1-1,0 1 0,0 0 0,-1 16 0,6-26-31,0-1 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,0 0 1,1-1 0,-1 0 0,0 1-1,1-1 1,-1 0 0,1 0 0,-1 0-1,3-1 1,-3 1-5,14 0-86,-3 1 28,1-1 1,-1-1-1,0 0 1,1-1-1,24-6 1,-34 7 69,0-1 0,0 0 0,-1 0 0,1 0 0,0-1-1,-1 1 1,0-1 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1-1,0 1 1,0-1 0,0 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-7 0,3-48 36,-4 57-50,-5 15-275,-70 136-404,51-98-2677,2-2-4142,13-27-1325</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9193.83">5545 557 5987,'0'0'14422,"16"11"-14246,-16 8-16,-4 0 113,-12 0-257,-9-1 80,1-1-96,-1 2-929,0-5-1696,5-3-1345</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9798.02">5918 342 10181,'0'0'9348,"11"-14"-8364,33-46-410,-40 57-520,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,1 0 0,8 2 0,-8-1-48,-3-1-7,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 1 0,-1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 3 0,0-3 4,0 1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1-1 1,-1 1 0,0 0-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,-4 5 0,1-5 13,0 1 0,-1-1 0,0 0 0,0 0 0,0 0 1,-8 2-1,8-2-6,-1-1 0,0 1 0,1 0 0,0 0 0,-8 7 0,18-12-29,-1 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,0 0 0,6 4 0,-7-4 7,0 2 0,-1-1-1,1 0 1,0 0 0,-1 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,-1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,-1 0 1,1-1 0,-2 5 0,0-4 17,0 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0-1 1,1 1-1,-1-1 1,0 1-1,-1-1 0,1 0 1,0 0-1,0-1 1,-6 3-1,-9 2 30,0 0-1,0-2 1,-1 0-1,0 0 0,-24 0 1,-31-2-402,27-1-4877,36-1 343</inkml:trace>
@@ -23217,10 +23216,10 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">79 334 5378,'0'0'7342,"-1"-17"-6592,-3-56 29,4 71-619,0-1-1,0 1 0,-1 0 0,1-1 1,0 1-1,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,0 0 0,-3-4 1,0-5 2433,-1 22-2617,-6 37 119,-6 54-1,6-30-19,4-10-46,1 0 0,5 66 0,1-105-28,0-20 3,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0-1 0,1 1 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1 0,-1 0-1,1 1 1,0-1 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,3 0 0,-1 0 8,1 0 0,0-1 0,-1 0 0,1 1 0,0-2 0,-1 1 0,1 0 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,3-4 0,1-3 65,0-1 0,-1 0 0,0 0 0,-1-1 0,-1 0 0,0 0 0,0 0-1,-1 0 1,-1-1 0,0 0 0,2-18 0,-1-17-1120,-3-86-1,-3 68-4238,-2 82-4711</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="555.18">459 321 7523,'0'0'6910,"0"-8"-6600,0-6-234,1-2 110,-3 34-19,-5 25 741,-1 0-1,-27 80 1,-6 26-2232,37-127-1051,1 0-1,-1 34 0,4-48-1898</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="788.04">322 547 9044,'0'0'7059,"44"-28"-7059,-10 22 208,10 4-127,0-1-162,-5 0-655,0 3-1473,-10-3-1216,-4-2-657</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1067.88">741 282 3314,'0'0'10399,"1"-13"-9516,5-24-280,-4 25 4,-8 39-206,-19 73 877,14-64-1104,2 1 0,1 0 1,-5 75-1,11-65-1166,0-24-1380,1 0-3666</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1067.87">741 282 3314,'0'0'10399,"1"-13"-9516,5-24-280,-4 25 4,-8 39-206,-19 73 877,14-64-1104,2 1 0,1 0 1,-5 75-1,11-65-1166,0-24-1380,1 0-3666</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1208.2">646 580 4994,'0'0'8676,"102"-64"-8564,-63 59-112,0-4-1328,-5 1-2802,-5 2-2801</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1702.41">1031 402 4946,'0'0'8057,"-6"-7"-7326,4 5-704,1-1-1,-1 1 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 1 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0 0,1 1-1,-1-1 1,0 0-1,1 1 1,-1 0-1,0-1 1,0 1-1,1 0 1,-1 1-1,0-1 1,0 0 0,1 1-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 1 1,0-1 0,-3 3-1,-2 1 10,-1 0-1,1 0 0,0 0 1,0 1-1,0 0 1,1 1-1,0-1 0,0 1 1,0 0-1,1 1 1,0-1-1,1 1 0,0 0 1,0 0-1,1 1 1,0-1-1,0 1 0,1 0 1,0-1-1,0 1 1,0 16-1,2-24-52,0 1-1,-1-1 1,1 1 0,0-1-1,0 1 1,1-1-1,-1 1 1,0-1 0,0 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1-1-1,0 0 1,0 1 0,-1-1-1,1 0 1,0 0 0,0 0-1,0 1 1,0-1-1,3 1 1,-1 0-15,1-1 0,0 0 0,-1-1-1,1 1 1,0-1 0,0 1 0,-1-1 0,7-1 0,-3 1 52,-3 0-5,0 0 0,0-1 0,0 0 0,0 1 0,0-2 0,0 1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,4-7-1,-2 1 143,0-1 0,-1 1 0,0 0 0,0-1 0,-1 0 0,0 1 0,-1-1-1,1-17 1,-2 25 657,0 10-595,-5 51-111,2-44-108,2 1 1,0-1-1,2 31 0,-1-45-63,0 1 0,1-1 1,-1 1-1,1-1 0,0 1 0,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,2 1 0,42 4-4352,-45-5 4330,28 0-5099</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2032.17">1201 465 6723,'0'0'7878,"7"3"-7672,-3 0-182,0 0 0,0 1-1,0-1 1,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0-1,-1 8 1,2 15 306,0-14-298,-1 0 1,0 0-1,-3 24 1,2-35 25,1-1 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 1 1,1-1-1,-1 0 1,-3 2-1,5-3-5,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1-2 1,-6-26 410,12-31-524,-3 48 23,1-1 1,1 1-1,0 0 1,1 1-1,0-1 1,1 1-1,0 0 1,15-16-1,-1 3-531,2 1 0,32-24 0,-37 32-434,1 1 1,1 0-1,0 1 1,1 1 0,0 2-1,0 0 1,1 1-1,0 0 1,1 2-1,38-5 1,-14 10-3353</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2032.16">1201 465 6723,'0'0'7878,"7"3"-7672,-3 0-182,0 0 0,0 1-1,0-1 1,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0-1,-1 8 1,2 15 306,0-14-298,-1 0 1,0 0-1,-3 24 1,2-35 25,1-1 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 1 1,1-1-1,-1 0 1,-3 2-1,5-3-5,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1-2 1,-6-26 410,12-31-524,-3 48 23,1-1 1,1 1-1,0 0 1,1 1-1,0-1 1,1 1-1,0 0 1,15-16-1,-1 3-531,2 1 0,32-24 0,-37 32-434,1 1 1,1 0-1,0 1 1,1 1 0,0 2-1,0 0 1,1 1-1,0 0 1,1 2-1,38-5 1,-14 10-3353</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2372.99">2195 395 12246,'0'0'6549,"0"-5"-6010,0-17-189,0 16-30,0 20-96,-6 21 28,-2-1 0,-15 45 1,13-49-800,1 1 0,1 1 1,-5 46-1,12-48-2524,1-6-875</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2686.31">2174 320 10997,'0'0'2713,"2"-16"-1485,6-51-327,-8 65-878,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0-1,0 1 1,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 1-1,4-2 1,37-2 193,-31 4-183,1-1-28,0 1 1,0 0-1,0 1 0,0 0 0,22 5 1,-30-5-7,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1-1,-1 1 1,1 0 0,-1-1 0,1 1 0,-1 0-1,0 1 1,0-1 0,0 0 0,-1 1-1,1-1 1,-1 0 0,0 1 0,1 4 0,0-2 9,-1 0 1,0 0-1,0 1 1,0-1-1,-1 1 1,0-1-1,-1 1 0,1-1 1,-1 0-1,0 1 1,-1-1-1,1 0 1,-1 0-1,0 0 1,-1 0-1,0 0 1,0 0-1,-3 5 1,-6 4 51,0-1 0,0 0 1,-2-1-1,-25 19 0,21-16-1052,0 0 0,-21 23 0,23-18-4262</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3058.87">2439 538 9620,'0'0'4789,"20"3"-4575,64 9 34,-81-11-233,0 0 1,0 1 0,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 1 0,0-1-1,0 1 1,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,-1 0 1,-1 3 0,-2-1 25,1-1 1,-1 1 0,-1-1-1,1 0 1,0 0 0,-1-1-1,0 0 1,0 0 0,0 0 0,0-1-1,-7 3 1,0-1 359,1-1 0,-1 0 0,0 0 0,-25 0 0,38-23 653,2 11-1048,1 0-1,-1 1 1,1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,1 0 0,0 1-1,1 0 1,-1 0 0,10-8 0,13-13-418,42-31-1,-69 58 394,11-8-631,0 0 0,0 1 0,1 0 0,15-6-1,-20 11-437,0 0 0,0 0 0,0 1-1,0 0 1,11-1 0,10 2-3402</inkml:trace>
@@ -23257,7 +23256,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">23 136 352,'0'0'2513,"0"-28"-466,0 25-2861</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1136.59">51 70 3682,'0'0'6005,"0"-8"-3220,-2 27-2656,0-1-1,-1 1 0,-1-1 0,-9 24 0,-8 42 240,19-68-583,-1 2 1340,5-42-218,2 10-884,0-1 0,1 1 1,0-1-1,1 1 0,1 1 1,12-20-1,-2 3-18,-17 28-20,1 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,3 0 0,-2 2-2,-1-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 1 1,-1-1-1,1 3 1,5 12-5,-2 0 0,0 1 0,3 21 0,-7-33 11,7 26 169,2-25-46,6-17-51,0-6-55,0-2 0,-2 0 0,0 0 1,-1-1-1,0-1 0,8-24 0,-14 141-35,-7-63 86,0-21-323,0-1 1,1 0-1,0 0 1,4 19 0,2-22-2078,7-7-2771</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1136.58">51 70 3682,'0'0'6005,"0"-8"-3220,-2 27-2656,0-1-1,-1 1 0,-1-1 0,-9 24 0,-8 42 240,19-68-583,-1 2 1340,5-42-218,2 10-884,0-1 0,1 1 1,0-1-1,1 1 0,1 1 1,12-20-1,-2 3-18,-17 28-20,1 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,3 0 0,-2 2-2,-1-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 1 1,-1-1-1,1 3 1,5 12-5,-2 0 0,0 1 0,3 21 0,-7-33 11,7 26 169,2-25-46,6-17-51,0-6-55,0-2 0,-2 0 0,0 0 1,-1-1-1,0-1 0,8-24 0,-14 141-35,-7-63 86,0-21-323,0-1 1,1 0-1,0 0 1,4 19 0,2-22-2078,7-7-2771</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1475.14">431 194 4466,'0'0'6568,"-9"17"-5949,-27 50-336,34-64-273,0 0 1,1 0-1,-1-1 0,1 1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 5 1,1 2-5,39-11 13,-37 0 5,-1 0-1,1-1 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0-1-1,0-3 1,2-6 436,-1-1 0,0 0-1,-1-24 1,-1 37-460,0 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1 0 1,0 0 0,1-1 0,-1 1-1,0 0 1,1 0 0,-1-1 0,0 1-1,1 0 1,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1 0-1,0 1 1,1-1 0,-1 0 0,1 1-1,-1-1 1,0 1 0,-2 0-238,1-1 1,-1 1-1,1 0 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,-2 3-1,-1 9-3048,4 0-575</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2420.64">691 212 6659,'0'0'8113,"-10"-3"-7886,6 1-225,1 1 1,0 0-1,-1 0 0,1 0 1,-1 1-1,1-1 0,0 1 1,-1-1-1,0 1 0,1 1 1,-1-1-1,1 0 0,0 1 1,-1-1-1,1 1 1,-1 0-1,1 0 0,0 1 1,-1-1-1,1 1 0,0-1 1,0 1-1,0 0 0,1 0 1,-1 0-1,0 1 0,1-1 1,-1 1-1,1-1 1,0 1-1,0 0 0,0 0 1,-2 4-1,1-3-15,1 0 1,-1 1-1,1-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,1 0 1,0 10-1,0-15 22,1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,1-1 0,24-6 238,-17 2-259,-1 0 1,0-1-1,0 0 1,-1 0-1,0-1 1,0 0-1,0 0 1,-1-1-1,0 1 0,-1-1 1,8-15-1,-6 9 17,0 0-1,-1-1 0,-1 0 0,-1 0 0,0 0 0,3-25 0,-7 38-15,3-25 60,-5 21-28,-4 17-104,-1 12 84,0-1 0,1 1 0,1 0-1,2 1 1,0-1 0,1 43 0,2-65-2,0 1 0,0-1 1,1 1-1,-1-1 0,0 0 1,1 1-1,-1-1 1,0 0-1,1 0 0,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,2 1 15,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,7 0 0,-4 0 22,1 0 0,-1-1-1,0 0 1,1 0 0,-1-1-1,0 0 1,1-1 0,10-2 0,-15 2-27,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1-1 1,-1 1-1,0-1 0,-1 1 0,1-1 0,0 0 0,-1 0 1,0-1-1,1 1 0,1-4 0,-2 0 65,0 1 0,0-1 0,-1 1 0,1-1 0,-2 0 0,1 1 0,-1-13 1,0 18 407,-2 1-476,0 1-1,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,1 1-1,-2 2 1,0 3-73,0-1 0,1 1 0,-1 0 1,1 0-1,0 11 0,6-17-24,0 0 0,0 0 0,0-1 1,0 0-1,0 0 0,9-1 0,-12 1 71,7-1-47,0 0 0,0-1-1,0 0 1,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0-1 0,-1 0 0,0-1 0,1 0 0,-2 0 0,1 0 0,-1-1 0,11-13-1,-10 9 45,0 1 0,0-1 0,-1 0 0,0 0 0,-1 0 0,-1-1 0,1 0 0,-2 0 0,0 0 0,0-1-1,-1 1 1,0-19 0,-1 30 50,-1 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0-1 0,0 2-22,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 1 1,1-1 0,-1 0 0,0 0-1,0 0 1,1 1 0,-1-1-1,1 0 1,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1-1-1,1 1 1,-1 0 0,-4 4-27,0 0 0,1 1 0,0-1 0,0 1 0,-4 9 0,-4 14 9,1 0 0,2 1 0,1 0 0,2 1 0,0 0 0,2 0 0,0 48 0,4-78 2,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1-1 0,0 1 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,1 1-1,2 0-47,0 0-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,6-2-1,2 0-494,-1 0-1,0-1 1,0-1 0,0 0-1,14-7 1,14-14-4189</inkml:trace>
 </inkml:ink>
@@ -23457,7 +23456,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">230 79 5603,'0'0'7334,"1"-9"-6889,2-3-247,3-31 799,-7 43-911,1-1-1,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,0 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 1,-36 0 686,25 1-508,8-1-223,-1 1 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,-6 7 0,-5 7 130,1 0-1,-14 21 1,22-28-98,1-2-39,1 0 1,0 0-1,0 0 1,1 1-1,0-1 1,1 1-1,0 0 0,0 0 1,1 0-1,0 0 1,0 0-1,2 9 1,0-17-26,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,3-1 0,0 1 22,2-1-25,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,0 0 0,1-1 0,-1 0 0,0 1 0,-1-2 0,1 1 0,-1 0 0,5-6 0,7-10-19,-1 0 0,22-40 0,-30 49 14,-5 9-2,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,1-6 0,-2 8 278,-6 24-333,4-18 62,-7 16 48,1 1-1,1 0 1,1 0 0,1 1-1,1 0 1,-3 38 0,8-60-47,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,1 0-1,-1-1 1,0 1 0,0 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,0-1 1,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1-1,1-1 1,51-5 107,-40 1-162,1-1 0,-1 0 0,0 0 0,16-12 1,22-19-3879,-47 30 991,-4-1-1108</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="931.35">522 43 6419,'0'0'6179,"12"5"-5160,-10 0-814,-1 1-1,0-1 1,0 1-1,0 0 1,-1-1 0,0 1-1,0 0 1,0-1 0,-2 8-1,1 7 466,0-14-521,0-1 1,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1-1-1,-1 1 1,1-1 0,-1 0-1,1-1 1,-1 1-1,-5 3 1,9-7-122,-1 0 1,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0-1,1-1 1,0 1 0,0 0-1,-1-1 1,1 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,0-1-1,0 1 1,0 0 0,0-1-1,-1 1 1,1-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,1 1 1,-1 0 0,0-1-1,0 0 1,2-19 49,0 13-79,0-1-1,1 1 0,0-1 1,0 1-1,1 0 0,-1 0 1,2 1-1,-1-1 0,1 1 1,0 0-1,0 0 0,1 0 1,-1 1-1,1 0 1,0 0-1,13-7 0,-9 6-19,1 0-1,0 1 1,0 1-1,0 0 1,0 0-1,1 1 1,0 0-1,-1 1 1,1 0 0,16 1-1,-26 1 18,-1 1 1,1-1-1,-1 0 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 1,0 1-1,2 60 393,-2-50-196,0-9-157,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 0 1,-1-1 0,1 1-1,-1-1 1,1 0 0,-1 0-1,-4 4 1,6-7 240,1-3-165,1-4-190,0-1 0,1 1 0,0-1 0,0 1-1,0 0 1,1 0 0,0 0 0,0 0-1,1 0 1,0 1 0,0-1 0,1 1-1,-1 0 1,1 1 0,1-1 0,-1 1-1,1 0 1,0 0 0,9-5 0,-5 2-16,0 2 1,1-1 0,0 2 0,0-1-1,1 2 1,-1-1 0,1 1 0,0 1-1,0 0 1,0 1 0,20-1 0,-31 5 81,0-1 0,0 1 0,-1 0 0,1-1 1,0 1-1,-1 0 0,1 0 0,-1-1 0,0 1 0,0 0 1,0 0-1,1 0 0,-2-1 0,1 1 0,0 0 1,0 0-1,-1 3 0,0-2 16,-1 8 52,0-1-1,-1 1 0,-1-1 1,0 0-1,0 0 0,-1 0 0,0-1 1,-12 17-1,10-15 116,0 1 1,0-1-1,1 1 1,1 1-1,-8 22 1,13-35-169,0 0 1,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,20-11-388,17-20-2106,-14 3-2146,-2-2-3971</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="931.34">522 43 6419,'0'0'6179,"12"5"-5160,-10 0-814,-1 1-1,0-1 1,0 1-1,0 0 1,-1-1 0,0 1-1,0 0 1,0-1 0,-2 8-1,1 7 466,0-14-521,0-1 1,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1-1-1,-1 1 1,1-1 0,-1 0-1,1-1 1,-1 1-1,-5 3 1,9-7-122,-1 0 1,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0-1,1-1 1,0 1 0,0 0-1,-1-1 1,1 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,0-1-1,0 1 1,0 0 0,0-1-1,-1 1 1,1-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,1 1 1,-1 0 0,0-1-1,0 0 1,2-19 49,0 13-79,0-1-1,1 1 0,0-1 1,0 1-1,1 0 0,-1 0 1,2 1-1,-1-1 0,1 1 1,0 0-1,0 0 0,1 0 1,-1 1-1,1 0 1,0 0-1,13-7 0,-9 6-19,1 0-1,0 1 1,0 1-1,0 0 1,0 0-1,1 1 1,0 0-1,-1 1 1,1 0 0,16 1-1,-26 1 18,-1 1 1,1-1-1,-1 0 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 1,0 1-1,2 60 393,-2-50-196,0-9-157,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 0 1,-1-1 0,1 1-1,-1-1 1,1 0 0,-1 0-1,-4 4 1,6-7 240,1-3-165,1-4-190,0-1 0,1 1 0,0-1 0,0 1-1,0 0 1,1 0 0,0 0 0,0 0-1,1 0 1,0 1 0,0-1 0,1 1-1,-1 0 1,1 1 0,1-1 0,-1 1-1,1 0 1,0 0 0,9-5 0,-5 2-16,0 2 1,1-1 0,0 2 0,0-1-1,1 2 1,-1-1 0,1 1 0,0 1-1,0 0 1,0 1 0,20-1 0,-31 5 81,0-1 0,0 1 0,-1 0 0,1-1 1,0 1-1,-1 0 0,1 0 0,-1-1 0,0 1 0,0 0 1,0 0-1,1 0 0,-2-1 0,1 1 0,0 0 1,0 0-1,-1 3 0,0-2 16,-1 8 52,0-1-1,-1 1 0,-1-1 1,0 0-1,0 0 0,-1 0 0,0-1 1,-12 17-1,10-15 116,0 1 1,0-1-1,1 1 1,1 1-1,-8 22 1,13-35-169,0 0 1,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,20-11-388,17-20-2106,-14 3-2146,-2-2-3971</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -23516,10 +23515,10 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">25 105 10149,'0'0'7067,"4"-16"-5763,1-6-884,11-45 948,-15 91 517,0 8-1804,-4 50-1,-18 9 97,13-66-148,2 1-1,1-1 1,1 1 0,0 27-1,9-51-23,0-1 0,0 1 0,0-1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 1,9-1-1,-4 1-10,115-1-926,-122 0 846,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 0 0,0 1 0,-1-1 0,1 0 0,0-1 0,-1 1 1,1 0-1,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 1,1-1-1,-1-1 0,2-4 0,4-10-360,0 0-1,5-32 0,-7 32 434,4-33 944,-9 80-764,-9 119 421,9-147-582,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,2 0 0,38 2 148,-34-3-140,0 1-74,-1 0 0,1-1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0-1 0,-1 1 0,1-1 0,0 0 1,-1-1-1,0 1 0,1-1 0,-2 0 0,1-1 0,5-5 0,5-7-177,-1-1 0,-1-1 0,15-29 0,-18 31 315,-14 31 106,0 0 1,2 0 0,0 0 0,0 1-1,1-1 1,1 1 0,2 21 0,-2-35-189,1 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0 0 0,0 0 0,-1 0-1,1-1 1,0 1 0,0 0 0,0-1-1,1 1 1,-1-1 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,1 0 0,-1 0-1,2 0 1,37 0-366,-28 0 186,4 0-273,-1-2 0,1 1-1,-1-2 1,1 0 0,-1-1 0,22-8-1,-29 9 257,0 0-1,0-1 0,-1 0 0,0 0 0,0-1 0,0 0 1,0 0-1,-1 0 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1 1 1,4-9-1,-1-11 1235,-11 21 739,-8 14-1112,3 1-352,-4 3 195,0 1 0,1 1 1,-10 16-1,19-26-444,-1 0-1,1 0 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,1-1 1,1 1-1,-1 0 1,1-1-1,0 1 1,0 0-1,2 7 1,-1-12-54,-1 0 1,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,1 0 0,1 0 0,36 0 40,-25 0-61,0-1-218,0 0 1,-1-1 0,1 0 0,-1-1-1,1 0 1,-1-1 0,0-1 0,0 0-1,-1 0 1,23-15 0,-25 14-28,-1-1 0,0 1 0,-1-2 0,1 1 0,-2-1 0,1-1 0,-1 1 0,0-1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,7-19 0,-6 5 574,-1 0-1,-1 0 0,-1 0 1,-2 0-1,0-26 2148,-2 82-2167,-12 54 87,7-55-251,1 0 0,0 37 0,0 20-1968,21-89-6813,3-8 4143</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="312.21">1244 228 3762,'0'0'10372,"1"-10"-9043,0 10-1323,-1-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 0 1,-127 65 524,127-64-489,1 1-47,2 0 37,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,5 1-1,-4-1 4,23 9 39,1-1 0,0-2 0,30 4 0,3-6-6399,-55-5 2056</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="312.2">1244 228 3762,'0'0'10372,"1"-10"-9043,0 10-1323,-1-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 0 1,-127 65 524,127-64-489,1 1-47,2 0 37,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,5 1-1,-4-1 4,23 9 39,1-1 0,0-2 0,30 4 0,3-6-6399,-55-5 2056</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="807.9">1424 245 2513,'0'0'10312,"1"-4"-9528,-1 4-730,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 36 1112,0-27-964,-1-1 0,0 1 0,0 0 1,0-1-1,-1 1 0,-1-1 0,0 0 1,-5 12-1,8-20-175,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,1-19 385,0 13-426,0 0 0,1 0-1,-1 0 1,1 1-1,0-1 1,3-5 0,0 3-52,1 0 0,0 0 0,0 1 0,1 0 1,0 0-1,1 0 0,-1 1 0,1 0 0,0 0 1,0 1-1,1 0 0,0 1 0,0 0 0,0 0 1,0 1-1,1 0 0,-1 1 0,1 0 0,-1 0 1,20 0-1,-28 3 80,0 1-1,0 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 2 1,1 0 25,0 115 93,2-118-464,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,3-1 0,-4 1 46,4-1-344,1 0 0,-1 0 1,0-1-1,0 1 0,0-1 0,-1 0 0,1 0 1,0-1-1,-1 1 0,1-1 0,-1 0 1,6-5-1,-5 3-49,20-12-2793</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1679.81">1811 236 2769,'0'0'10624,"-3"-3"-9546,3 2-1047,0 0 0,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 1-1,1-1 1,-1 1-1,1-1 0,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,1 0-1,-1 0 0,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 1,0 0-1,1 0 0,-2 1 1,0 0 35,0 1 1,0-1-1,1 1 0,-1 0 1,0 0-1,1-1 0,0 1 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 0 0,-1 4 1,-2 6 275,1 0 0,0 0 0,1 1 0,0-1 0,1 1 0,0 18 0,2-29-318,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,2 0 0,42-7 379,-42 6-388,0-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 0 1,0-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,-1-1-1,0 1 0,0-1 1,0 0-1,-1 0 1,1-3-1,0 4-18,-1 1 1,1 0-1,-1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,-1-1 0,1 1 1,-1 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 0,-1 1 1,1-1-1,-1 0 1,0 0-1,0 0 0,-2-1 1,-21-3-522,18 5-1095,20-1 800,35-4 507,-37 3 316,1 1-1,0 1 1,-1 0-1,21 1 1,-30 1 7,-1-1 1,0 1 0,1 0-1,-1-1 1,0 1 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 1-1,1-1 1,-1 0 0,1 1-1,-1-1 1,1 3 0,6 39 473,-6-37-352,0 11 199,4 22 335,-5-38-647,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,-1 0-1,1-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 1 0,0-1-1,0 0 1,0 0 0,1 1 0,-1-1-1,1 0 1,5-1-10,0 1-1,0-1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0 0,0-1-1,0 0 1,11-8-1,59-48-162,-36 25-87,-25 27 254,-8 11 43,-7 24 87,-1-11-109,1-6 3,-1-9-19,1 0 0,0 1 1,0-1-1,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 1,-1 1-1,1-1 0,1 4 0,0-5-5,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0-1 0,-1 0-1,1 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,2-1 1,4 1 8,0-1 1,0 0-1,0-1 0,0 0 1,0 0-1,-1-1 0,1 0 0,-1 0 1,1-1-1,-1 0 0,0 0 1,0 0-1,-1-1 0,1 0 1,-1-1-1,0 1 0,-1-1 1,1 0-1,-1-1 0,4-7 1,-4 7-19,0 0 0,0-1 0,-1 0 1,-1 0-1,1 0 0,-1-1 0,-1 1 1,1-1-1,-2 1 0,1-1 0,-1 0 1,0 0-1,-1 0 0,0 0 0,0 0 1,-1 1-1,0-1 0,-4-14 1,4 20-11,-1 1 1,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-4 0 0,-5-2-73,-1 2-1,1 0 1,-1 0 0,-16 2-1,26-1-71,1 0 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 1 0,0 0 0,0 0 0,0 0 0,-1 0-1,1 1 1,0-1 0,-2 3 0,-20 23-5572,12-7-2429</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2267.22">2766 267 9188,'0'0'6801,"-3"6"-5937,0-2-525,-1 1 66,1-1 0,0 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,-2 9 0,32-30 694,-27 14-1084,1 1-1,-1-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0-3 1,-1 4-11,1 0 0,0 0 0,-1 0 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,-2 1-1,-3-1-10,1 0 0,-1 1 0,0-1 0,0 1 0,1 1 0,-8 1 1,12-2-2,-1-1 1,1 1 0,-1-1 0,1 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,1 0 0,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1-1,1 2 1,25-5 52,-19 1-32,-1-1 1,1 0 0,-1-1-1,1 1 1,-1-1-1,10-5 1,-13 7-7,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1-2 0,-1 3-140,-1 0 1,0 1-1,0-1 1,0 1-1,-1 0 1,1-1 0,0 1-1,0 0 1,0 0-1,0 0 1,-3 1-1,3-1-120,-22 4-2475,-1 6-1387</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2267.21">2766 267 9188,'0'0'6801,"-3"6"-5937,0-2-525,-1 1 66,1-1 0,0 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,-2 9 0,32-30 694,-27 14-1084,1 1-1,-1-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0-3 1,-1 4-11,1 0 0,0 0 0,-1 0 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,-2 1-1,-3-1-10,1 0 0,-1 1 0,0-1 0,0 1 0,1 1 0,-8 1 1,12-2-2,-1-1 1,1 1 0,-1-1 0,1 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,1 0 0,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1-1,1 2 1,25-5 52,-19 1-32,-1-1 1,1 0 0,-1-1-1,1 1 1,-1-1-1,10-5 1,-13 7-7,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1-2 0,-1 3-140,-1 0 1,0 1-1,0-1 1,0 1-1,-1 0 1,1-1 0,0 1-1,0 0 1,0 0-1,0 0 1,-3 1-1,3-1-120,-22 4-2475,-1 6-1387</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -23548,9 +23547,9 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">20 174 3490,'0'0'7446,"1"-4"-6491,2-1-490,1-5-144,-3-1 5707,-1 21-5844,-20 244 362,17-224-524,2-19-306,-3 21-712,3-11-6573</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="309.4">29 214 8628,'0'0'3450,"0"-16"-2218,-1-6-738,0 4 330,0 0 0,1-1 1,4-33-1,-3 48-777,1 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0-1,1 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0 0 0,5-1-1,5-1-47,0 0-1,1 1 0,-1 1 1,28 0-1,-39 2-69,0-1 0,0 1-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,-1 0 0,1 0-1,0-1 1,-1 1 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 1-1,-1-1 1,1 1 0,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 5 0,0 1-858,0 0 1,0-1 0,-1 1 0,0 0 0,-1 0 0,0 0 0,0 0-1,-3 16 1,-9 8-6902</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="309.39">29 214 8628,'0'0'3450,"0"-16"-2218,-1-6-738,0 4 330,0 0 0,1-1 1,4-33-1,-3 48-777,1 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0-1,1 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0 0 0,5-1-1,5-1-47,0 0-1,1 1 0,-1 1 1,28 0-1,-39 2-69,0-1 0,0 1-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,-1 0 0,1 0-1,0-1 1,-1 1 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 1-1,-1-1 1,1 1 0,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 5 0,0 1-858,0 0 1,0-1 0,-1 1 0,0 0 0,-1 0 0,0 0 0,0 0-1,-3 16 1,-9 8-6902</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="496.74">49 389 8196,'0'0'7027,"15"0"-6915,14 0 64,5 0-176,5-6-512,5 6-1233,-5 0-2401</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1236.11">453 383 10981,'0'0'5960,"0"0"-5928,-1-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,-1 1 1,1-1 0,0 0-1,0 1 1,-1-1-1,1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0-1-1,2 3-23,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,1 1-1,-1 0 1,-1-1 0,1 1 0,0 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0-1-1,0 5 1,1-1 21,-1 1 1,1-1-1,-1 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,0-1 1,0 0-1,-3 6 0,-11 6 344,14-17-344,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 1,1-2-18,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 1,0 0-1,0-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 1,2-2-1,3-3-302,0 1 0,0-1 1,1 1-1,0 1 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 1 0,1 0 0,12-2 1,13-3-2802,54-4 1,-57 9 1372,41-5 7257,-81 22-1805,4-4-3583,0 0-1,1 0 1,0 0 0,0 0-1,2 1 1,-1 0 0,1 0-1,-2 11 1,7-21-137,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,0-1-1,1 0 0,-1 1 1,0-1-1,1 0 1,-1 0-1,1 1 1,-1-1-1,0 0 0,1 0 1,-1-1-1,1 1 1,-1 0-1,0 0 1,3-1-1,36-7 190,-34 5-178,-1-1-1,1 0 0,-1 0 1,0 0-1,0-1 1,0 1-1,-1-1 0,7-8 1,-9 10-11,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,-1-1 0,1 1 0,-1-5 0,0 6-29,1 1 1,-1 0-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,-1 1 0,1-1 0,0 1 1,-1-1-1,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,-2 0 0,-3 1-448,1-1 0,0 1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,-6 5 0,-2 8-2310,7-4-2174</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1236.1">453 383 10981,'0'0'5960,"0"0"-5928,-1-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,-1 1 1,1-1 0,0 0-1,0 1 1,-1-1-1,1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0-1-1,2 3-23,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,1 1-1,-1 0 1,-1-1 0,1 1 0,0 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0-1-1,0 5 1,1-1 21,-1 1 1,1-1-1,-1 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,0-1 1,0 0-1,-3 6 0,-11 6 344,14-17-344,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 1,1-2-18,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 1,0 0-1,0-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 1,2-2-1,3-3-302,0 1 0,0-1 1,1 1-1,0 1 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 1 0,1 0 0,12-2 1,13-3-2802,54-4 1,-57 9 1372,41-5 7257,-81 22-1805,4-4-3583,0 0-1,1 0 1,0 0 0,0 0-1,2 1 1,-1 0 0,1 0-1,-2 11 1,7-21-137,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,0-1-1,1 0 0,-1 1 1,0-1-1,1 0 1,-1 0-1,1 1 1,-1-1-1,0 0 0,1 0 1,-1-1-1,1 1 1,-1 0-1,0 0 1,3-1-1,36-7 190,-34 5-178,-1-1-1,1 0 0,-1 0 1,0 0-1,0-1 1,0 1-1,-1-1 0,7-8 1,-9 10-11,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,-1-1 0,1 1 0,-1-5 0,0 6-29,1 1 1,-1 0-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,-1 1 0,1-1 0,0 1 1,-1-1-1,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,-2 0 0,-3 1-448,1-1 0,0 1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,-6 5 0,-2 8-2310,7-4-2174</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1891.38">947 328 6099,'0'0'7328,"16"-6"-6781,51-20 6,-66 25-528,-1 1 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 1,-1-1-1,1 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 1 0,-1 30 595,-1-24-353,2 8 59,0-12-228,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 1 0,0 0 0,1-1 0,-5 7 0,4-18 412,6-8-662,2 6-20,1 0-1,0 0 1,1 1 0,0 0 0,0 0 0,1 1 0,16-13 0,-19 16 136,0 1 1,0 0-1,0 1 0,0 0 1,0 0-1,1 0 1,-1 1-1,1-1 1,0 2-1,0-1 1,0 1-1,0 0 1,0 0-1,11 1 0,-17 1 40,0-1 0,0 0 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,-1-1-1,1 1 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 2 0,0 40 257,-1-30-138,1-5 47,0 1 0,-1-1 0,0 1 0,-1-1 0,0 1 0,-5 15 0,11-31-141,0 0 0,1 1 1,0 0-1,0-1 0,1 2 0,0-1 1,0 1-1,9-6 0,64-45-1522,-72 51 1395,1 1 1,-1 0-1,1 0 0,-1 1 1,1 0-1,0 0 0,0 1 1,1 0-1,13-2 1,-21 5 91,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 1,0 0-1,0 0 0,-1 2 1,1 35 302,0-29-121,0-1-62,-1-3-4,1 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,2 8 0,-2-11-78,0-1 0,-1 0 1,1 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-2 0,1 1 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 1,0 1-1,1-1 0,-1 0 1,1 0-1,0 0 0,-1 0 1,3 0-1,12 0-85,-1-2 0,0 1 0,0-2-1,1 0 1,-2-1 0,1 0 0,0-1 0,14-8 0,-7 2-1746,-1-1 0,25-17 0,0-9-8795</inkml:trace>
 </inkml:ink>
 </file>
@@ -23643,7 +23642,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">180 95 6723,'2'-5'13814,"1"-21"-13179,-4 3-57,1 23-572,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,-10 35 149,6-19-228,-4 21 99,2 0-1,2 0 1,0 50-1,1-7-855,1-66-123,1 0-1,-2 0 1,-5 18-1,-12 12-6234,6-29 1961</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="280.77">0 527 8500,'0'0'9079,"26"0"-7769,49 2-1199,38-1-677,-40-8-2872,-46 0-721,-14-2-2596</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="619.35">85 39 1313,'0'0'14950,"-54"-39"-12148,74 39-3010,18 0 192,21 0-32,4 0-1217,1 0-752,-16 0-144,-9 6-4466</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="619.34">85 39 1313,'0'0'14950,"-54"-39"-12148,74 39-3010,18 0 192,21 0-32,4 0-1217,1 0-752,-16 0-144,-9 6-4466</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -23677,9 +23676,9 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1024.9">586 85 720,'0'0'16357,"0"-11"-11429,-1 27-4950,-1 1 0,-1-1 0,-6 23 0,5-23-12,0 1 0,1 0 0,-1 25 0,0-22-2734,-7-14-5371,2-6 530</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1511.78">469 183 11877,'0'0'5712,"11"-1"-5600,38-3-282,-26 3-767,0-1 0,0 0 0,32-9-1,-27-8 1194,-26 11 1427,-17 8-1197,-70 22-265,66-15-337,-1-1-1,0-1 1,-1-1 0,0-1-1,-21 1 1,23-4-82,19-1 206,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 1,1-1-1,-1 1 65,1-1-3,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0-1,1-1 1,-1 1 0,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 1-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 1-1,-1-1 1,1 1-1,0-1 1,3 2-1,2 2-342,0 1 0,0 0 0,0 0 0,-1 0 0,11 10 0,2 2-2098,-5-8-2415</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1861.07">1015 52 7603,'0'0'11918,"0"-4"-11078,-2 52-177,0 76-236,1-45-9206</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2078.28">961 161 12854,'0'0'6467,"10"-5"-6515,14 5 48,10 0 0,0 0-448,0 0-465,-4 0-575,-1 0-673,-5 0-1505,-9-3-1392</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2078.27">961 161 12854,'0'0'6467,"10"-5"-6515,14 5 48,10 0 0,0 0-448,0 0-465,-4 0-575,-1 0-673,-5 0-1505,-9-3-1392</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2400.09">1237 139 4946,'0'0'10400,"-16"-2"-9917,-3-2-391,13 3-66,-1-1 0,1 1 0,0 0 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 1-1,-1 0 1,1 0 0,0 0 0,-10 4 0,-16 6-68,6-2-200,-1 0 0,1-2 0,-1 0 0,-1-2 0,-38 2 0,68-32-457,-1 23 728,0-1-1,1 1 0,-1 0 1,1 0-1,-1 0 1,1 0-1,0 1 0,0-1 1,-1 0-1,1 1 1,0-1-1,1 1 0,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 1 1,1-1-1,-1 1 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,4 2-1,4 3 31,-1-1 1,1 1-1,-1 1 0,-1 0 1,17 14-1,-9-8-275,18 5-4589,-14-13-1854</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4107.27">1534 208 5394,'0'0'10010,"6"11"-5944,-5-11-4042,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1 0 0,1-1-1,-1 1 1,0 0 0,1-1 0,-1 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1 0,0 1-1,0-1 1,1 1 0,-1-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,-20 10-93,19-8 68,-2 2-8,0-1-1,0 1 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,-2 8 0,4-11-37,20-8-455,-20 8 499,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,-13 11-17,11-10 12,1 0 0,-1 1-1,1-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 3 0,3-5 3,1 0 0,0 0 1,0 0-1,-1-1 1,1 1-1,0-1 0,-1 0 1,1 0-1,-1-1 0,8-2 1,-2-1-374,5-2 471,-7 1-6340</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4107.26">1534 208 5394,'0'0'10010,"6"11"-5944,-5-11-4042,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1 0 0,1-1-1,-1 1 1,0 0 0,1-1 0,-1 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1 0,0 1-1,0-1 1,1 1 0,-1-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,-20 10-93,19-8 68,-2 2-8,0-1-1,0 1 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,-2 8 0,4-11-37,20-8-455,-20 8 499,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,-13 11-17,11-10 12,1 0 0,-1 1-1,1-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 3 0,3-5 3,1 0 0,0 0 1,0 0-1,-1-1 1,1 1-1,0-1 0,-1 0 1,1 0-1,-1-1 0,8-2 1,-2-1-374,5-2 471,-7 1-6340</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -23708,7 +23707,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">130 3 3105,'0'0'8463,"0"-2"-7726,0 5-479,-2 19 77,-1 0 0,0-1 0,-2 1 0,-1-1 0,-8 22 0,-10 35 136,14-33-232,5-15-105,-2-1-1,-1 0 1,-2-1 0,-23 50-1,34-91 842,9-55-955,11 8-497,38-77 0,-48 116 432,0 2 1,2 0-1,0 0 0,1 2 0,0-1 0,2 2 1,24-21-1,-40 36 46,1 0 1,0 0-1,-1 0 1,1 0-1,0 1 0,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 1-1,3 10 30,0 0 0,-1-1-1,-1 1 1,0 13 0,0-9 53,6 308 913,-7-235-665,-1-78-249,-2-12-1162,-4-16-3677,0-1-1233</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="325.46">66 359 6275,'0'0'10178,"0"0"-10153,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 1,0 0-1,8-2 50,-1 0-1,1 1 1,-1 0-1,1 0 1,0 1 0,-1-1-1,1 2 1,10 1-1,6-1 34,-19-1-246,95-5 1351,-50-8-1785,-45 11-89,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,6-6 0,-1 1-6036</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="325.45">66 359 6275,'0'0'10178,"0"0"-10153,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 1,0 0-1,8-2 50,-1 0-1,1 1 1,-1 0-1,1 0 1,0 1 0,-1-1-1,1 2 1,10 1-1,6-1 34,-19-1-246,95-5 1351,-50-8-1785,-45 11-89,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,6-6 0,-1 1-6036</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -23863,7 +23862,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1037.07">1355 426 6675,'0'0'3834,"10"-19"-2991,1 1-670,0 0 108,-1-1 0,0 0 0,-1 0 0,-2-1 0,8-24 0,-10 18 360,-1 1 0,-2-1 0,0 0-1,-1 0 1,-6-49 0,5 74-589,-1 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 1 0,0-1 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,-2 1 0,-40 14-150,31-7 106,1 1 0,0 0 1,0 1-1,0 0 0,2 1 0,-1 0 0,1 0 1,1 1-1,0 0 0,1 0 0,0 1 0,1 0 0,0 1 1,1-1-1,0 1 0,1 0 0,-2 17 0,4-16-6,0 0-1,0-1 0,2 1 0,0 0 1,1-1-1,0 1 0,1 0 0,0-1 0,2 1 1,-1-1-1,2 0 0,0 0 0,1-1 0,0 1 1,1-1-1,16 23 0,5-3 32,-19-25-12,-1 1 1,-1 1 0,1 0-1,-1 0 1,-1 0-1,8 17 1,-14-26-7,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,-1 1 0,1-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 1 0,1-1 0,0 0 0,-1 0 1,1 0-1,-1 1 0,1-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-2 0 0,-31-1 845,24 1-663,3 0-405,-9 0 589,0 0 0,-1-2 0,-15-2 0,27 3-525,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,-7-4 0,9 5-162,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,1 1-1,-1-1 1,0 1 0,1 0-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1 0,0-2-1,0-5-6454</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1411.59">1500 733 5987,'0'0'8481,"20"-3"-7350,62-11-285,-74 11-764,0 0 0,0 0-1,0-1 1,-1 0 0,1-1 0,-1 1 0,-1-1 0,1-1 0,-1 1-1,1-1 1,-1 0 0,-1-1 0,0 1 0,1-1 0,-2 0 0,1 0 0,-1-1-1,3-8 1,0 3 138,0-1 0,-1 0-1,-1 0 1,0 0 0,-1-1-1,-1 0 1,0 0-1,1-28 1,-5 54-223,0 0 1,-1 0-1,-1 0 0,1 0 0,-8 15 0,6-14 33,0-1 0,1 1 0,0 0 0,1 0 0,-2 19 0,4-27-26,0-1 0,-1 0 0,2 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,3 5 0,-3-6-90,1-1 0,-1 0 0,1 1 0,-1-1-1,1 0 1,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1-1-1,1 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 0-1,-1 1 1,4-2 0,-2 1-335,0 0-1,0-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-1 1-1,0-1 1,0 0-1,4-6 1,17-23-5510</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1549.48">1911 292 6787,'0'0'12390,"-29"-31"-12502,24 45-1793,0 11-400,0 9-4578</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2464.18">1872 515 5987,'0'0'12376,"17"2"-11397,55 8-272,-69-9-650,1 1-1,-1-1 1,1 0-1,-1 1 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,-1-1-1,2 4 1,-1 4 62,1-1-1,-1 1 1,-1 0-1,0 0 1,0 15 0,-4 16 226,2-30 260,0-32 982,2 11-1629,-1 0 0,2 0 1,-1 0-1,2 0 0,-1 1 0,1-1 0,0 1 1,1-1-1,0 1 0,0 0 0,0 1 1,1-1-1,1 1 0,-1 0 0,1 0 1,0 0-1,1 1 0,7-6 0,-4 4-578,1 0 0,0 1-1,0 0 1,0 1 0,1 0 0,0 1-1,0 0 1,0 1 0,1 0-1,-1 1 1,1 0 0,16 0 0,81-1-6797,-44 8 15289,-78-3-3049,4 0-4725,1 0-1,-1 1 0,0 0 0,1 0 0,0 0 1,-1 1-1,1 1 0,0-1 0,-7 5 0,5 0-56,1 0 0,0 0 0,0 1 0,0 0 0,1 0 0,-10 18 0,14-21-43,0 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,1 1 1,0-1 0,0 1-1,0-1 1,1 1-1,0-1 1,0 1 0,1 8-1,0-14-4,0 1 1,0-1-1,1 1 0,-1-1 0,0 0 1,0 1-1,1-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 0,1 1 1,-1 0-1,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,0 0 1,1-1-1,50-5-98,-45 3 175,1-1-1,-2-1 1,1 1-1,0-1 0,-1-1 1,0 1-1,0-1 0,-1 0 1,8-10-1,-9 11-5,-1 0 1,0 0-1,0 0 1,-1-1-1,1 0 1,-1 0-1,0 0 0,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 0,0-10 1,-2 16 211,0 34-482,-1-26 196,1 0 0,1 0 0,-1 0 0,1 0 1,0 0-1,1 0 0,4 12 0,-5-18 1,1 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1-1 0,1 1 0,0-1-1,0 0 1,5 0 0,-1 1 20,0-1 0,0 0 0,0 0-1,0 0 1,0-1 0,-1 0 0,1-1 0,0 1 0,0-1-1,-1 0 1,1-1 0,-1 0 0,0 0 0,0 0-1,0-1 1,0 0 0,0 0 0,-1 0 0,0-1 0,0 0-1,0 0 1,0 0 0,-1 0 0,0-1 0,0 0 0,0 0-1,-1 0 1,0 0 0,3-8 0,-1-1 13,-4 11-19,1 0 0,-1-1 0,1 1 0,0 0 0,0 0 1,1 0-1,-1 0 0,6-6 0,-7 24-761,-21 416 187,20-423 527,-1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,-1 1 0,1-2 0,-1 1 0,-1-1 0,1 0 0,0 0 0,-1-1 0,0 1 0,0-2 0,0 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 0 1,1 0-1,-1-1 0,1 0 0,-14-4 0,17 4-321,1 0 0,0 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 0 0,1 0 1,-4-3-1,-24-31-5649</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2464.17">1872 515 5987,'0'0'12376,"17"2"-11397,55 8-272,-69-9-650,1 1-1,-1-1 1,1 0-1,-1 1 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,-1-1-1,2 4 1,-1 4 62,1-1-1,-1 1 1,-1 0-1,0 0 1,0 15 0,-4 16 226,2-30 260,0-32 982,2 11-1629,-1 0 0,2 0 1,-1 0-1,2 0 0,-1 1 0,1-1 0,0 1 1,1-1-1,0 1 0,0 0 0,0 1 1,1-1-1,1 1 0,-1 0 0,1 0 1,0 0-1,1 1 0,7-6 0,-4 4-578,1 0 0,0 1-1,0 0 1,0 1 0,1 0 0,0 1-1,0 0 1,0 1 0,1 0-1,-1 1 1,1 0 0,16 0 0,81-1-6797,-44 8 15289,-78-3-3049,4 0-4725,1 0-1,-1 1 0,0 0 0,1 0 0,0 0 1,-1 1-1,1 1 0,0-1 0,-7 5 0,5 0-56,1 0 0,0 0 0,0 1 0,0 0 0,1 0 0,-10 18 0,14-21-43,0 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,1 1 1,0-1 0,0 1-1,0-1 1,1 1-1,0-1 1,0 1 0,1 8-1,0-14-4,0 1 1,0-1-1,1 1 0,-1-1 0,0 0 1,0 1-1,1-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 0,1 1 1,-1 0-1,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,0 0 1,1-1-1,50-5-98,-45 3 175,1-1-1,-2-1 1,1 1-1,0-1 0,-1-1 1,0 1-1,0-1 0,-1 0 1,8-10-1,-9 11-5,-1 0 1,0 0-1,0 0 1,-1-1-1,1 0 1,-1 0-1,0 0 0,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 0,0-10 1,-2 16 211,0 34-482,-1-26 196,1 0 0,1 0 0,-1 0 0,1 0 1,0 0-1,1 0 0,4 12 0,-5-18 1,1 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1-1 0,1 1 0,0-1-1,0 0 1,5 0 0,-1 1 20,0-1 0,0 0 0,0 0-1,0 0 1,0-1 0,-1 0 0,1-1 0,0 1 0,0-1-1,-1 0 1,1-1 0,-1 0 0,0 0 0,0 0-1,0-1 1,0 0 0,0 0 0,-1 0 0,0-1 0,0 0-1,0 0 1,0 0 0,-1 0 0,0-1 0,0 0 0,0 0-1,-1 0 1,0 0 0,3-8 0,-1-1 13,-4 11-19,1 0 0,-1-1 0,1 1 0,0 0 0,0 0 1,1 0-1,-1 0 0,6-6 0,-7 24-761,-21 416 187,20-423 527,-1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,-1 1 0,1-2 0,-1 1 0,-1-1 0,1 0 0,0 0 0,-1-1 0,0 1 0,0-2 0,0 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 0 1,1 0-1,-1-1 0,1 0 0,-14-4 0,17 4-321,1 0 0,0 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 0 0,1 0 1,-4-3-1,-24-31-5649</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2617.99">2671 89 10885,'0'0'6931,"73"-6"-7219,-53 42-2113,4 9-4610</inkml:trace>
 </inkml:ink>
 </file>
@@ -23893,7 +23892,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">31 60 9012,'0'0'1417,"0"19"-1132,-23 225 1236,17-154 2673,6-93-3220,0-45-351,-1 0-426,6-55-1,-4 90-177,1-1 0,1 1 0,0 0 0,1-1 0,0 2 0,1-1 0,0 0 0,14-21 0,-18 32-32,-1 1 0,1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0 0 1,1-1-1,-1 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 1 0,0 0 0,2-1 0,-2 2-8,0 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 3 0,4 17 20,0 1 0,-2-1 0,1 31 0,4 31 85,56-278 719,-61 185-825,1-1 0,0 0 0,1 1-1,0 0 1,1 0 0,0 1 0,0-1-1,12-11 1,-18 20 8,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,1 1-1,-1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 1-1,1 17-120,-1-12 59,4 106 40,-4-59 227,11 75 1,-10-123-179,1 1-1,-1 0 1,1 0-1,0-1 1,0 1-1,1-1 1,5 9 0,-7-12 6,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,-1-1 1,1 1 0,-1-1-1,3-1 1,9-7-63,-1 0 0,1-1 1,-2-1-1,0 0 1,17-21-1,6-5-3106,-12 16-991,-6 6-2610</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.83">607 87 5907,'0'0'11533,"-1"-16"-11029,-3 34-386,0 0-1,2 1 0,0-1 1,1 1-1,1-1 1,1 1-1,3 24 0,-2-39-103,-1-1 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1-1 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,5 0 1,-4 0 10,-1 0-1,1-1 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1-1-1,-1 1 0,1 0 1,-1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0-1 1,4-4-1,0-4 144,0-1-1,0 0 1,-1-1-1,-1 1 1,0-1-1,-1 0 1,0-1-1,-1 1 1,2-21-1,-9 109-172,-23 128 0,9-91-22,8-37 85,-3-2 0,-3 1-1,-42 115 1,56-184-50,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,-1-1 0,-6 8 0,10-11 5,-1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0-1 0,-5-8-1,-1 0-1,2-1 1,-1 1 0,2-1-1,-1 0 1,2 0 0,-1-1-1,1 1 1,-1-19 0,1 9-196,2 0 0,0 0 1,1 0-1,6-36 0,-4 49-33,0 0-1,1 0 0,0 0 0,0 1 0,1-1 1,0 1-1,0 0 0,1 0 0,0 0 0,0 0 0,0 1 1,10-9-1,9-6-2327,50-34 0,-72 53 2420,69-45-5669</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.82">607 87 5907,'0'0'11533,"-1"-16"-11029,-3 34-386,0 0-1,2 1 0,0-1 1,1 1-1,1-1 1,1 1-1,3 24 0,-2-39-103,-1-1 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1-1 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,5 0 1,-4 0 10,-1 0-1,1-1 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1-1-1,-1 1 0,1 0 1,-1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0-1 1,4-4-1,0-4 144,0-1-1,0 0 1,-1-1-1,-1 1 1,0-1-1,-1 0 1,0-1-1,-1 1 1,2-21-1,-9 109-172,-23 128 0,9-91-22,8-37 85,-3-2 0,-3 1-1,-42 115 1,56-184-50,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,-1-1 0,-6 8 0,10-11 5,-1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0-1 0,-5-8-1,-1 0-1,2-1 1,-1 1 0,2-1-1,-1 0 1,2 0 0,-1-1-1,1 1 1,-1-19 0,1 9-196,2 0 0,0 0 1,1 0-1,6-36 0,-4 49-33,0 0-1,1 0 0,0 0 0,0 1 0,1-1 1,0 1-1,0 0 0,1 0 0,0 0 0,0 0 0,0 1 1,10-9-1,9-6-2327,50-34 0,-72 53 2420,69-45-5669</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -23956,8 +23955,8 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 593 10389,'0'0'4845,"2"-1"-4807,0 1 1,0 0 0,0 0-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 0 0,0 1-1,-1-1 1,4-3 0,24-45 206,28-65-1,-41 78-193,2 0-1,1 1 1,1 1-1,50-62 1,-24 48 18,3 2 0,54-40 1,-102 86-79,-1 0 0,0-1 0,1 1 0,-1 0 1,0 0-1,1-1 0,-1 1 0,0 0 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,1-1 0,-1 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,0 1 0,1-1 1,-1 0-1,0 1 0,0-1 0,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,0 33-171,0-26 284,-4 103 690,-21 118-1,15-79-498,10-104-6598,0-68 965</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="308.49">162 296 11509,'0'0'4853,"3"0"-4485,34 0 15,1-2 0,-1-1-1,0-2 1,0-2 0,0-1-1,48-17 1,-75 20-299,1 0 90,-1 3-7379</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.84">1315 169 2273,'0'0'10015,"-19"-7"-9689,-63-20-137,78 25-176,-1 1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 1 0,1-1 0,-1 0 0,-5 8 0,-2-1 46,-4 4 21,0 1 0,0 1 0,2 1 0,0 0 0,1 0 0,1 2 0,1-1 0,0 1-1,1 1 1,1-1 0,1 1 0,1 1 0,1-1 0,1 1 0,0 0 0,2 0 0,0 1 0,2 31-1,1-50-79,-1-1 1,1 1-1,-1 0 0,1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 0 1,1-1-1,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,3 0 0,9 1 673,-1 0-1,1 0 0,29-2 0,-27-1 613,-16 1-1237</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="308.48">162 296 11509,'0'0'4853,"3"0"-4485,34 0 15,1-2 0,-1-1-1,0-2 1,0-2 0,0-1-1,48-17 1,-75 20-299,1 0 90,-1 3-7379</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.83">1315 169 2273,'0'0'10015,"-19"-7"-9689,-63-20-137,78 25-176,-1 1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 1 0,1-1 0,-1 0 0,-5 8 0,-2-1 46,-4 4 21,0 1 0,0 1 0,2 1 0,0 0 0,1 0 0,1 2 0,1-1 0,0 1-1,1 1 1,1-1 0,1 1 0,1 1 0,1-1 0,1 1 0,0 0 0,2 0 0,0 1 0,2 31-1,1-50-79,-1-1 1,1 1-1,-1 0 0,1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 0 1,1-1-1,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,3 0 0,9 1 673,-1 0-1,1 0 0,29-2 0,-27-1 613,-16 1-1237</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1304.99">1798 139 6627,'0'0'6342,"-21"-2"-5753,-70-2-279,83 5-251,0 1 1,0 0 0,1 0-1,-1 1 1,1 0 0,0 0-1,0 1 1,0-1 0,0 2-1,0-1 1,1 1 0,0 0-1,0 0 1,0 1 0,1-1-1,0 1 1,-7 10 0,8-11 0,-9 11 17,1 1 1,1 1 0,1 0-1,1 0 1,0 1 0,1 0-1,1 0 1,1 1 0,0 0 0,2 0-1,0 0 1,2 1 0,0-1-1,1 1 1,3 36 0,-1-54-79,0 1 1,0 0-1,0 0 1,0-1 0,1 1-1,-1 0 1,1-1-1,0 0 1,0 1 0,0-1-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1-1 1,1 1 0,1-1-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1-1 0,0 1-1,-1-1 1,1 0-1,0 0 1,4 0-1,10 2 56,0-1 0,0-1 0,0-1-1,29-3 1,-38 2-133,-1-1 0,0 0-1,0-1 1,-1 0 0,1 0 0,-1 0 0,1-1-1,-1 0 1,0-1 0,0 1 0,-1-1-1,1-1 1,-1 1 0,6-8 0,10-7-2847,-3 4-3048</inkml:trace>
 </inkml:ink>
 </file>
@@ -24016,7 +24015,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 9 11157,'0'0'12614,"5"-7"-11048,-5 15-1560,1 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,1-1 0,0 1 1,0-1-1,1 0 1,0 0-1,5 7 0,-7-11-29,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 1,3-2-1,-1 0 9,-1 0 1,-1-1 0,1 1 0,0-1 0,-1 0-1,0 0 1,0-1 0,0 1 0,0 0 0,-1-1-1,0 0 1,0 0 0,0 1 0,0-1 0,1-7-1,12-26-44,-14 35 56,-1 3-20,0 29-202,-2-6 291,0 1-1,-1-1 1,-12 39-1,-1 15-5073,15-65-80</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="480.17">587 74 6867,'0'0'8876,"-15"-19"-6942,13 19-1894,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1-1,0-1 1,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-3 1-1,3 1-33,0 0 0,1-1 1,-1 1-1,0 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,1 4 0,-1-4-2,1 1 0,0-1 0,0 1-1,0-1 1,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,1 1 1,-1-1 0,1 0 0,0 1 0,3 1 0,-3-2 4,0 0-1,0 0 1,0 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,-1 1-1,0-1 1,0 0 0,0 0-1,0 1 1,-1 0-1,1-1 1,-1 1 0,0 0-1,0-1 1,1 7 0,-3-9 0,1 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,-2 0 0,-16 2-1596,5-3-3862</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="587.46">587 61 11045</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="587.45">587 61 11045</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="682.18">587 61 11045,'10'-50'2161,"0"48"-704,0-4-289,9 3-688,10 3-335,5 0-129,-4 0-16,9 0-353,-5 3-1423,-5 3-4659</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1188.3">1482 35 11685,'0'0'6227,"-10"-2"-5851,5 1-333,0 0-1,0 0 0,0 1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,1-1 0,-1 2 0,0-1 0,0 0 1,0 1-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,-5 7 0,0-1 97,1 1 0,0-1-1,0 1 1,-9 21 0,14-26-134,0-1 1,0 0-1,1 1 0,-1 0 0,1-1 1,0 1-1,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 1,1 0-1,-1 0 0,1-1 1,2 7-1,-2-9-40,1-1-1,-1 1 1,1 0 0,0 0 0,0-1 0,-1 1-1,1-1 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,2 1-1,0 0-112,0-1 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0-1 0,7-1 0,-11 1 155,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-2 0,-1 1 24,1 0 0,0 0-1,-1 0 1,1 0 0,-1 1 0,0-1-1,1 0 1,-1 0 0,0 0 0,0 0-1,-1 1 1,1-1 0,-2-1 0,-4-1-160,0 2 1,0-1-1,-1 1 1,1 0-1,-1 0 1,1 1 0,-1 0-1,0 0 1,1 1-1,-1 0 1,0 1-1,1-1 1,-9 3-1,10 2-2683</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1635.6">1737 94 2081,'0'0'15879,"-4"-2"-14868,2 1-874,-12-6 194,14 7-323,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,69-1 46,80 2 52,-147-1-109,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0 0 1,-1 0 0,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0-1,1 1 1,-1 1 14,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 1,1-1-1,0 0 0,-1 1 0,-1 3 0,-2 2 42,0 1 0,0 0 0,-1-1 0,0 0 0,-6 8 0,-3 1-373,-31 41 930,27-15-5459,17-36-7</inkml:trace>
@@ -24077,7 +24076,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">8 95 9108,'0'0'6769,"-1"-5"-5758,0-2-704,-4-37 3199,5 42-3474,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,1-1 0,-1 1 0,0 0-1,1-1 1,-1 1 0,1 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,1-1 0,-1 0 0,0 1-1,2-1 1,3-1-33,-1 1-1,1 0 1,-1 0 0,1 1-1,-1-1 1,1 1-1,0 1 1,-1-1-1,1 1 1,-1 0 0,7 1-1,-10-1-1,0 1 1,1-1-1,-1 0 0,0 1 1,0-1-1,0 1 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 1-1,0-1 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1 0 1,-1-1-1,0 1 0,0-1 0,0 1 1,0 4-1,-5 58 19,4-62-26,0 1 1,1-1-1,-1 0 1,-1 0-1,1 0 1,0-1-1,-1 1 1,1 0-1,-1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,-1 0-1,1 0 1,-5 3-1,7-5 10,0 0 1,0 0-1,0-1 0,0 1 0,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 1,20 3 23,36-2-718,-46-1 236,75-1-5819,-45-3 69</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1037.34">713 39 6403,'3'-3'14905,"9"1"-14296,118 2-697,-129 0 117,-2 3-278,-1 0 242,0 0 1,0 1-1,0-1 1,0-1-1,0 1 1,-1 0-1,1 0 1,-4 2-1,-5 7 72,8-7-70,-1-1-1,0 1 0,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 0,0-1 1,-9 5-1,20-8-93,1 0-1,-1 1 0,0 0 1,0 0-1,0 1 0,0 0 1,0 0-1,-1 0 0,1 1 1,0 0-1,-1 0 0,0 0 1,0 0-1,0 1 0,0 0 1,6 6-1,-11-9 102,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0-1 0,-1 1 0,0 0 1,-32 5 21,27-5 0,-148 6-681,121-7-1223,32 2 1672,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1-1,-2-2 1,-3-12-5842</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1037.33">713 39 6403,'3'-3'14905,"9"1"-14296,118 2-697,-129 0 117,-2 3-278,-1 0 242,0 0 1,0 1-1,0-1 1,0-1-1,0 1 1,-1 0-1,1 0 1,-4 2-1,-5 7 72,8-7-70,-1-1-1,0 1 0,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 0,0-1 1,-9 5-1,20-8-93,1 0-1,-1 1 0,0 0 1,0 0-1,0 1 0,0 0 1,0 0-1,-1 0 0,1 1 1,0 0-1,-1 0 0,0 0 1,0 0-1,0 1 0,0 0 1,6 6-1,-11-9 102,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0-1 0,-1 1 0,0 0 1,-32 5 21,27-5 0,-148 6-681,121-7-1223,32 2 1672,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1-1,-2-2 1,-3-12-5842</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -24143,8 +24142,8 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">54 671 12886,'0'0'10375,"5"-16"-9353,-4 25-1175,-1 1-1,-1 0 1,1-1 0,-1 1-1,-1-1 1,0 1-1,0-1 1,-1 0-1,0 0 1,-1 0 0,-8 17-1,5-15-1090,-10 20-6164,11-17-2412</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1078.16">356 172 7123,'0'0'11958,"1"-4"-11027,1-6 156,-3 13-122,-7 28-120,-1 13-2632,5-11-4059,4-24 126</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1310.35">369 172 8900,'98'-56'2481,"-98"51"-576,5 2 2033,-5 6-3842,0 16-16,0 4 304,0 2-352,0 0 16,0-3-48,-5 3-1200,-10-3-721,0-2-1137,1-6-3633</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1078.15">356 172 7123,'0'0'11958,"1"-4"-11027,1-6 156,-3 13-122,-7 28-120,-1 13-2632,5-11-4059,4-24 126</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1310.34">369 172 8900,'98'-56'2481,"-98"51"-576,5 2 2033,-5 6-3842,0 16-16,0 4 304,0 2-352,0 0 16,0-3-48,-5 3-1200,-10-3-721,0-2-1137,1-6-3633</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2145.29">678 317 6643,'0'0'7668,"4"-5"-6729,5-7-1073,6-4 5431,-11 20-3016,-2 15-2199,-4 10 107,-1-1 0,-9 39 0,-1 10-28,1-36 766,3-14-3623,6-8-8805</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2413.01">688 258 9476,'0'0'9893,"4"-16"-9797,1 16-96,5 0 0,5 0 0,4 0 288,1 0-288,-6 0-16,1 11-976,0 6-977,-15 2-432,0 1-2770,0-1-3009</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2630.96">559 595 12422,'0'0'6867,"34"3"-6867,1-3 16,-1 0-16,5 3-1681,-5-3-960,-5 0-2642</inkml:trace>
@@ -24632,7 +24631,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">40 65 8212,'0'0'8425,"0"-10"-7550,0-44 1940,0 70-2599,-3 89 119,-22 149-1,14-164 192,50-90-542,-5 0-124,1 0 0,0-3 0,0-1 0,-1-1 1,1-2-1,58-20 0,-88 25 103,0 0 1,0 0 0,0 0-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,0-1 1,-1 0 0,7-8-1,-7 6 30,-1 0-1,1 0 1,-1 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,-1 0-1,0-10 1,0 15 2,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,-1-1 1,0 0-1,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,-1 0 1,1 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 2 0,-3 11 23,0-1 1,1 1-1,1 0 0,1 0 0,0 0 1,0 0-1,1 0 0,3 16 1,-2-28-15,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0-1 0,0 1 0,1-1 0,3 1 0,7 1 10,1-1 1,0 0-1,16-2 0,-12 1 0,-9-1-20,0-1 0,-1 0 0,1 0 0,-1 0 1,1-1-1,-1-1 0,0 1 0,0-1 0,-1-1 0,1 1 1,-1-1-1,0-1 0,0 1 0,0-1 0,10-12 0,-1 0-205,-1 0-1,0-1 0,-2-1 0,20-37 0,-26 39 113,-1 0 0,-1-1-1,0 0 1,-2 1 0,0-1-1,-1-1 1,-1 1 0,-3-34-1,2 24 136,0 27-29,-6 41-208,-8-8 313,1 0-1,1 0 1,2 1 0,-12 62 0,-4 136 609,20-187-678,-11 50 0,-3 12 63,20-69-147,0-35 38,1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 0,1 0 1,3-2-86,0 0 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1 1 1,0-1-1,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1-1 0,1 0 1,1-6-1,1-2-246,-2 1 0,1-1 0,-2 1-1,0-1 1,1-24 0,-3 33 224,0-12-190,0 0-1,-1 0 0,-1 1 0,0-1 1,-5-17-1,5 29 326,1 1 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,0 1 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 1,-1 0-1,0 1 1,0 0-1,0-1 1,0 1-1,0 1 1,0-1-1,-1 1 1,1-1-1,-7 0 0,-17 1 375,27 1-455,1 1 34,0-1 0,1 1 0,-1-1 0,0 0 1,0 1-1,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,13 1 33,-1-1-1,1 0 1,-1-1-1,1-1 1,-1 0-1,0-1 1,0 0-1,0-1 1,0 0-1,-1-1 1,0-1-1,0 0 1,0 0-1,0-1 1,14-12-1,-17 12 23,-1 0 1,0-1-1,0 0 1,0-1-1,-1 0 0,-1 0 1,1 0-1,-1-1 1,-1 0-1,0 0 1,0 0-1,-1-1 0,-1 1 1,0-1-1,0 0 1,-1 0-1,0 0 0,0-20 1,-1-1 461,0 11 522,-3 41-761,-3 33-228,-1 5 328,4 110 1,2-164-368,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1-1 0,1 1 0,0 0 0,1-1 0,5 4 0,-4-4-497,-1-1-1,0 1 1,0-1 0,0 0-1,1-1 1,-1 1 0,1-1-1,-1 0 1,0 0 0,1 0-1,-1-1 1,0 1 0,8-3-1,3-4-5373</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="185.71">829 343 7860,'0'0'10084,"-15"-5"-10004,30 2-48,9-3 144,11 3-176,-1-2-1312,5 2-1057,-10-5-3826</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="185.7">829 343 7860,'0'0'10084,"-15"-5"-10004,30 2-48,9-3 144,11 3-176,-1-2-1312,5 2-1057,-10-5-3826</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="494.2">1274 1 10565,'0'0'8036,"-5"3"-7810,-4 6-117,-1 0-1,1 1 1,1 0-1,0 1 1,0-1-1,1 1 1,-10 22-1,-37 93 859,52-121-940,-20 55 290,-20 83-1,35-114-290,2-1 0,2 1 0,0 0 1,2 0-1,4 40 0,-3-64-235,1 0 1,0 1-1,0-1 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,0 0-1,0-1 0,0 0 0,1 1 0,-1-1 1,1 0-1,0-1 0,0 1 0,0-1 1,1 0-1,-1 0 0,1 0 0,0 0 1,9 3-1,30 10-3790</inkml:trace>
 </inkml:ink>
 </file>
@@ -24665,7 +24664,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="284.11">113 110 7668,'0'0'6723,"-3"-3"-6390,3 3-324,0 0-1,-1-1 0,1 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0-1,1-1 0,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,0-1 0,0 1 1,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,1-1-1,-1 1 0,0 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,35-13 979,10 7-1682,-9 7-3971,-27 4 67</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="792.67">364 237 3153,'0'0'2100,"20"-4"7295,-9-1-9871,9-10 726,-16 13-229,0 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1-1 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 1,0-1-1,1-4 0,-3 9-12,1-1 1,-1 1-1,1-1 0,-1 0 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 0,1 0 1,-1 0-1,0 0 0,0-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0 0 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 0,0 0 1,1 0-1,-1 1 1,0-1-1,1 0 0,-1 1 1,-1 0-1,-30 13 134,28-8-136,0-1 0,0 1 0,1 0 0,0 0 1,0 1-1,0-1 0,1 0 0,0 1 0,0 0 0,0 0 0,1-1 0,0 1 1,1 0-1,-1 0 0,1 0 0,1 0 0,1 10 0,-2-15-81,1 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,3 1 0,51 3-3845,-51-4 3413,30 0-4390</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="995.68">681 131 6515,'0'0'9828,"0"3"-9876,-5 17 48,-4 2 64,-1 0 17,-5-2-65,6-4-16,-6-4-1153,5-1-528,-4-11-1408,4 0-1233,0 0-1409</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1163.64">681 131 4194,'-126'39'11205,"130"-22"-11221,11 3 96,5-4-160,-1-5 80,1 1-1104,4-7-1137,0-5-3186</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1163.63">681 131 4194,'-126'39'11205,"130"-22"-11221,11 3 96,5-4-160,-1-5 80,1 1-1104,4-7-1137,0-5-3186</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1379.09">785 70 11365,'0'0'3794,"0"42"-3762,0-23-32,0-2-48,0-3-448,0-6-1009</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1520.36">785 70 9941,'64'-67'4818,"-64"76"-4930,0 10 48,0 9-593,0-3-2256,0-3-1153</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1953.37">15 3 7411,'0'0'6820,"-5"-3"-6644,0 12-144,5 8 80,-4 5 0,4 3-64,0 3-96,14-3-801,20 0-2592,10 0-2706</inkml:trace>
@@ -24698,7 +24697,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">49 64 9316,'0'0'12022,"-49"-45"-11398,49 54-672,0 16 48,0 2 80,5 4-80,5 0-336,10-3-1265,4-6-1200,0-8-369,6-6-2832</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="159.14">239 17 13430,'0'0'7540,"0"-16"-7668,0 41-817,0 11-1232,0 3-1296,0-3-4275</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="159.13">239 17 13430,'0'0'7540,"0"-16"-7668,0 41-817,0 11-1232,0 3-1296,0-3-4275</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="774.68">351 128 7684,'0'0'12181,"-5"2"-11895,2 0-271,0 0 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 1,1-1-1,-1 7 0,-18 78 291,15-59-153,-8 34 93,4 0 0,-4 108 1,10-148-143,-4-30 106,-6-38 89,9-3-281,2 0-1,2-1 1,2 1 0,11-63-1,-8 86-26,1-1-1,18-44 0,-20 60-10,0 0-1,1 0 1,0 1-1,1 0 0,0 0 1,0 0-1,1 1 1,0 0-1,14-13 0,-19 19 7,0 1-1,0-1 0,0 0 0,0 1 1,0-1-1,1 1 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 1 0,0-1 1,-1 1-1,1 0 0,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1 0 1,1 0-1,2 1 0,-2 1 3,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 0,-1 1 1,1 0-1,-1-1 0,0 1 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 4 0,1 1-17,-1 0 0,1 0-1,-2 0 1,1 0-1,-2 0 1,1 0-1,-1 0 1,0 0-1,-1-1 1,0 1-1,0-1 1,-1 1 0,0-1-1,0 0 1,-1-1-1,0 1 1,-1-1-1,1 0 1,-1 0-1,-1-1 1,1 0-1,-1 0 1,0 0 0,-9 5-1,11-8-38,-1 3-174,-1-1-1,0 0 1,0 0 0,-1-1-1,1 1 1,-1-2-1,0 1 1,0-1-1,0 0 1,-10 1 0,23-2 265,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 1 0,-1-1 1,0 1-1,0 0 0,5 7 0,13 10 114,63 40-412,-26-29-3420,-28-19-1790</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1257.03">733 256 11669,'0'0'5947,"-6"24"-5245,-51 198 448,32-105-337,21-106-321,1-20 269,1-18-170,2 17-575,-1-19-2,1-1 0,2 1 0,1 0-1,12-52 1,-3 41-81,-5 10-20,1 0-1,2 1 1,1 1-1,1 0 0,2 0 1,19-30-1,-32 58 84,-1-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 1 0,11 36-58,-11-32 71,11 61 232,-3-1 0,0 97 0,-5-82-193,-3 25-880,-2-63-6822</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1958.98">712 485 12358,'0'0'4647,"15"-9"-3953,-5 2-711,1-1-200,1 1 0,-1 1 0,1 0 0,0 0-1,1 1 1,22-5 0,-24 7-479,1 0 1,-1-1-1,0 0 0,0 0 1,-1-1-1,12-8 0,-16 9 589,-1 0-1,0 0 1,0 0-1,0-1 1,-1 0-1,1 0 1,-1 0 0,-1 0-1,1-1 1,-1 1-1,0-1 1,4-9-1,4-14 3012,22-40 0,-30 72-50,3 21-2848,-3 20 697,-2-1-1,-5 66 1,4-107-685,-1-1 0,1 1 0,0 0 0,0-1-1,-1 1 1,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1 0 0,1-1 115,1-15 433,0-2-497,-1-1-69,1 0 0,0 0-1,2-1 1,0 1 0,0 0-1,2 0 1,0 1 0,7-17-1,-9 28-52,11-24-55,-13 28 101,1 1-1,-1-1 0,0 0 0,0 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 0,1 1 0,0-1 1,-1 1-1,1-1 0,-1 1 0,1-1 1,0 1-1,0-1 0,-1 1 0,1 0 1,0-1-1,0 1 0,-1 0 0,2-1 0,0 5-18,0-1-1,0 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,0 1 0,-1 0 1,1 0-1,-1 0 0,0 0 1,0 5-1,1 3 27,4 183 140,-5-132 74,0-70 80,0 2-275,0-1 0,0 1 0,0 0 1,1 0-1,0 0 0,0 0 0,0 0 1,1 0-1,3-9 0,8-14-179,1 1-1,1 1 1,1 0-1,2 1 1,0 0-1,41-40 1,-59 65 160,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1 0 0,1 0 0,6 45 189,-3 0 0,-1-1 1,-5 50-1,0 2-231,3-74-417,0 8-1818,0-11-2713</inkml:trace>
@@ -24826,7 +24825,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">88 10 10485,'0'0'6811,"0"-10"-1070,-2 36-5799,-1 0-1,-1-1 1,-8 30 0,-6 31 123,11-39 7,-25 90 0,29-128-74,-4 22-116,28-31 38,0-3 38,1-1-1,-1-1 1,1-1 0,-1 0-1,-1-2 1,0 0-1,0-2 1,25-15 0,-42 23 29,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,0 1 1,0-1-1,0 0 0,0 1 1,-1-1-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 1,0 0-1,1-1 0,-1 1 1,-1 0-1,1 0 0,0-1 1,-1 1-1,0 0 0,1 0 0,-1 0 1,0 0-1,-1 0 0,1 0 1,-3-4-1,-3-11 203,1 5 176,4 27-383,3 28 21,-2-1 0,-2 1 0,-1-1 0,-3 1 0,-14 52 0,11-64-156,-16 57-2028,19-29-5015,7-38-1305</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1115.09">723 102 9893,'0'0'5503,"0"-5"-5092,0-21 2463,-35 26-1935,27 1-941,1-1 1,-1 1-1,0 1 1,0-1 0,1 2-1,-1-1 1,1 1-1,0 0 1,-1 0 0,1 1-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1 0 1,0 1 0,1-1-1,0 1 1,0 0-1,0 0 1,0 1 0,1 0-1,0-1 1,0 1-1,-3 11 1,-2 3-4,2 1 0,0 0 0,1 0 0,1 1 0,1 0-1,1 0 1,1 37 0,1-51-18,1 0-1,1 1 1,0-1-1,0 0 0,1 0 1,0 0-1,0 0 1,6 13-1,-6-19 21,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0-1,1-1 0,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,1 0-1,-1 0 0,0 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,-1-1-1,1 0 1,4 0-1,-1 0-4,0 0-1,1-1 1,-1 1-1,0-1 1,0-1-1,0 1 1,0-1-1,0 0 1,0-1-1,0 0 1,6-4-1,-9 5 7,-1-1 0,0 0 0,0 1 1,0-1-1,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,0-8 0,0 12-7,0-1 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 1,1-1-1,-1 0 1,1 1-1,-1 0 0,1-1 1,-1 1-1,0-1 0,-21 0-34,4 2 125,17-1-178,25-3-3212,4-4 3059,-13 4 224,-1 0 0,0 0 0,27 0 0,-39 8 32,-1 1 0,1 0 0,-1-1 1,-1 1-1,1 0 0,-1 0 0,0 0 1,-2 9-1,2-7 136,0 165 412,5-154-4397</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1115.08">723 102 9893,'0'0'5503,"0"-5"-5092,0-21 2463,-35 26-1935,27 1-941,1-1 1,-1 1-1,0 1 1,0-1 0,1 2-1,-1-1 1,1 1-1,0 0 1,-1 0 0,1 1-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1 0 1,0 1 0,1-1-1,0 1 1,0 0-1,0 0 1,0 1 0,1 0-1,0-1 1,0 1-1,-3 11 1,-2 3-4,2 1 0,0 0 0,1 0 0,1 1 0,1 0-1,1 0 1,1 37 0,1-51-18,1 0-1,1 1 1,0-1-1,0 0 0,1 0 1,0 0-1,0 0 1,6 13-1,-6-19 21,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0-1,1-1 0,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,1 0-1,-1 0 0,0 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,-1-1-1,1 0 1,4 0-1,-1 0-4,0 0-1,1-1 1,-1 1-1,0-1 1,0-1-1,0 1 1,0-1-1,0 0 1,0-1-1,0 0 1,6-4-1,-9 5 7,-1-1 0,0 0 0,0 1 1,0-1-1,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,0-8 0,0 12-7,0-1 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 1,1-1-1,-1 0 1,1 1-1,-1 0 0,1-1 1,-1 1-1,0-1 0,-21 0-34,4 2 125,17-1-178,25-3-3212,4-4 3059,-13 4 224,-1 0 0,0 0 0,27 0 0,-39 8 32,-1 1 0,1 0 0,-1-1 1,-1 1-1,1 0 0,-1 0 0,0 0 1,-2 9-1,2-7 136,0 165 412,5-154-4397</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1885.09">1053 327 7603,'0'0'8468,"1"-3"-8075,0 1-68,1 11 85,-1 31 518,-6 56 317,2-68-988,1 45 0,2-58-145,0-14 262,-6-42 1128,3 8-1489,1-1-1,2 0 1,6-56 0,-4 78-20,0-1-1,1 1 1,1 0 0,0 0 0,0 1 0,1-1 0,1 1 0,-1 0 0,2 0 0,0 1 0,0-1 0,1 2 0,11-12 0,-14 16-5,1 1-1,-1 0 1,1 1 0,0-1-1,0 1 1,0 0 0,1 1-1,-1 0 1,1 0 0,-1 0 0,1 0-1,8 0 1,-15 40-340,-2-27 363,0 0 1,-1-1 0,0 1-1,-1 0 1,0-1-1,0 0 1,-1 0 0,-1 0-1,1 0 1,-2-1-1,-13 16 1,-26 47-293,45-71 181,0 0 1,0 1-1,0-1 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,3 2 0,2 1-318,1-1 0,0 0 0,0-1 1,0 0-1,0 0 0,11 2 0,-13-4 97,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 1 0,0-1 0,8 7 0,-12-8 324,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 0,0 0 1,0-1-1,0 1 0,-1-1 0,-45 21 2033,39-19-1953,-20 8 125,-1-2-1,0-1 1,0-1 0,-1-2 0,0 0-1,1-3 1,-43-2 0,56-3-4306,6-11-5576</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2979.16">1922 116 11509,'0'0'8049,"-3"-4"-7870,3 3-182,0 1 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 0,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 0,-1-1 0,1 1 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 1 0,1-1 1,-6 21-60,7 56 104,1-43 77,0 59-40,1-52-32,-3 0-1,-1 0 1,-1-1 0,-11 51-1,11-89 755,0-7-276,-2-21-81,-2-35-418,6 32-38,1-1 1,1 1 0,1 0-1,2 0 1,16-57 0,-17 76 1,0 0 0,0 1 1,1-1-1,1 1 0,-1 0 1,1 0-1,1 0 0,0 1 1,0 0-1,0 1 0,1-1 1,0 1-1,1 1 0,-1 0 1,1 0-1,0 0 0,1 1 1,0 1-1,19-7 0,-21 9-11,1 0 0,-1 1 0,0 0 0,0 0-1,11 1 1,-15 0-28,-4 0 31,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,-1 1 0,-7 25-152,-3-13 48,-2 0-1,0-1 1,0 0-1,-2-1 0,1-1 1,-1 0-1,-31 16 0,0 2-1041,37-22 832,6-5 164,0 0 0,0 1 0,0-1 0,0 0 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 0,-5 1 0,9 0 67,1-1 0,-1 0 1,1 1-1,-1-1 1,1 1-1,-1-1 0,1 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 1 1,1 0-1,33 31 479,-1 1-1,-2 2 1,-2 1-1,-1 1 1,39 69-1,-54-95-2167,-9-11-1772</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3521.61">2471 214 11461,'0'0'5974,"0"5"-5942,2 50 162,-2 67 488,-1-110-577,0-1 0,-1 1 0,-1-1 1,1 0-1,-2 1 0,1-1 0,-2-1 0,-5 12 0,10-22-56,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 1-1,0-23 149,1 22-181,0-18 2,0-20 23,1 0-1,8-51 1,-7 77-44,1 1 1,0-1 0,1 1 0,0 0 0,0 1-1,1-1 1,1 1 0,0 0 0,0 0-1,1 0 1,0 1 0,10-10 0,-14 16-4,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1 1 1,1-1-1,-1 0 0,0 1 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 0,-1 0 0,1-1 0,-1 1 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 1,-1 1-1,0-1 0,0 1 0,1 5 0,5 25 35,-3 0 0,0 1 0,-3 0 0,-2 35 0,1-22-9,0-39-75,-1 0 0,0 0 0,-1 1 0,1-1-1,-6 12 1,-8 10-2419,-8-9-4883,14-21-45</inkml:trace>
@@ -24863,7 +24862,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">2 380 12758,'0'0'6979,"-1"-5"-6205,1 5-743,0-1 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 1,0 0-1,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,1 0 1,-1 1-1,1-1 0,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 1 0,2-1 0,27-3 895,-6 2-953,-13 1-300,112-11 851,-81 10-4056,0 1-5045,-26 1 2385</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="464.42">457 294 9172,'0'0'8129,"3"-8"-7339,-2 5-731,1 0 1,-1-1-1,1 1 1,0 0-1,-1 1 1,1-1-1,1 0 1,-1 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,3-2 1,-1 1-12,0 1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 1 0,1-1 0,5 2 0,-10-2-50,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 1-1,1 7 9,-1-3 7,0 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,0-1 0,0 1 0,-4 3 0,-9 8 50,-1-1-1,-27 19 1,34-28-93,5-1 468,24-4-278,50 0-558,12 0-2182,-2-5-5258,-38-3-706</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="464.41">457 294 9172,'0'0'8129,"3"-8"-7339,-2 5-731,1 0 1,-1-1-1,1 1 1,0 0-1,-1 1 1,1-1-1,1 0 1,-1 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,3-2 1,-1 1-12,0 1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 1 0,1-1 0,5 2 0,-10-2-50,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 1-1,1 7 9,-1-3 7,0 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,0-1 0,0 1 0,-4 3 0,-9 8 50,-1-1-1,-27 19 1,34-28-93,5-1 468,24-4-278,50 0-558,12 0-2182,-2-5-5258,-38-3-706</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="793.26">874 57 8516,'0'0'10722,"-5"-10"-9919,-17-31-571,23 36-368,8 7 104,9 7 51,0 4 4,0 0-1,-1 2 1,-1 0-1,-1 0 1,0 2 0,-1 0-1,0 0 1,-2 1 0,0 1-1,-1 0 1,-1 1 0,15 40-1,-20-45-17,0 0 1,-2 0-1,0 0 0,0 1 0,-1-1 0,-1 1 0,-1-1 0,0 1 1,-1-1-1,-1 1 0,0-1 0,-1 1 0,-1-1 0,0 0 1,-1 0-1,-1-1 0,0 0 0,-1 0 0,-9 15 0,-4-2-216,-1-1-1,-1-1 0,-1-1 0,0-1 0,-47 34 0,11-16-3037,-100 53 1,61-43-3822</inkml:trace>
 </inkml:ink>
 </file>
@@ -24925,9 +24924,9 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="947.74">750 100 6883,'0'0'5747,"4"19"-6948,1 4-832,-5 2-832,10 0 208</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2046.35">920 259 1793,'0'0'8585,"8"-11"-6941,25-34-316,-33 45-1288,1-1-1,-1 1 1,0 0-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,0-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0-1 0,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,-2-1-1,-16 1 400,15 0-317,-5 1-67,1-1 0,-1 2 1,1-1-1,-1 1 0,1 0 0,0 0 1,0 1-1,0 0 0,0 0 1,0 1-1,1 0 0,-11 8 1,12-9-57,1 1 1,0-1 0,0 1-1,0 0 1,1 0 0,0 0-1,-1 1 1,1-1-1,1 1 1,-1-1 0,1 1-1,0 0 1,0 0 0,0 1-1,0-1 1,1 0 0,0 0-1,0 9 1,1-13-10,0 0 1,0-1-1,0 1 0,0-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,1-1 0,-1 0 1,0 1-1,1-1 1,-1 1-1,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,2 0 0,26 2-299,-21-2 277,1-1 0,-1 0 1,1 0-1,-1-1 0,8-3 0,0-3 171,-12 6-171,0 1 0,0-1 0,0 0-1,0 1 1,1 0 0,-1-1-1,0 1 1,1 1 0,6-2 0,-9 2 16,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 1 0,-1-1 0,1 0 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 2 0,1 34 63,0-1-1,-3 1 0,-10 62 0,9-81-55,-1 0-1,-1-1 0,0 1 1,-1-1-1,-1 0 0,-1-1 0,0 1 1,-1-2-1,-16 22 0,17-27 105,0-1-1,-1-1 0,0 0 1,0 0-1,-1 0 1,0-1-1,0-1 0,0 0 1,-1 0-1,0-1 0,0 0 1,-1-1-1,1 0 1,-1-1-1,-21 3 0,32-6-76,1-1 1,-1 1-1,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,1-1 0,2-29-484,0 25 305,-1 0-1,1 0 0,0 0 0,0 0 0,1 0 0,0 1 1,0 0-1,0-1 0,0 1 0,10-7 0,60-46-756,-55 45 804,56-40-637,79-61-745,-126 92 1463,-1-2 0,-2-1 0,28-34 0,-50 54 290,1 0-1,-2 0 1,1 0 0,0 0 0,-1-1 0,0 1 0,0-1 0,-1 1 0,1-1-1,-1 0 1,-1 1 0,1-1 0,-1-12 960,-11 35-1251,4-5 33,-56 108 161,57-107-140,1 1 0,0 0 0,1 0 1,0 1-1,2-1 0,-1 1 0,1 18 0,37-34-140,-17-5 140,1-1 0,-2-1 0,1-1 0,-1 0 0,0-1 0,-1-1 0,22-19 0,-38 30-44,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0-1,1 0 1,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1-1,0 0 1,0 1 0,0-1 0,1 0 0,-1 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,10 32 115,-3-8 55,-5-23-144,1 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0-1 0,1 1 1,-1 0-1,0-1 0,0 0 0,1 1 0,-1-1 1,0 0-1,5-1 0,1 0 25,-1 0 0,0 0 0,0 0-1,0-1 1,0 0 0,15-6 0,-15 2-49,1 0-1,-1 0 1,0 0 0,-1-1 0,0 0-1,0-1 1,0 0 0,-1 0-1,0 0 1,-1-1 0,0 0 0,0 0-1,-1 0 1,0-1 0,5-15 0,-2 0 338,-1 0 1,-1 0 0,-1-1 0,-2 0 0,0-27 0,-3 58-281,0 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 0 0,0 1 0,-3 3 0,-8 14 46,10-14-290,-42 95 735,29-48-1306,10-3-3317</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2214.49">1461 375 12598,'0'0'6259,"117"-66"-6259,-58 54-128,4-1-2354,5 1-223,-9-2-3426,-6-5 2578</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2451.76">2124 0 5298,'0'0'11283,"-19"12"-11014,10-6-231,-7 3 32,0 1-1,2 1 0,-1 0 0,1 1 1,1 0-1,0 1 0,-14 18 1,18-18 74,-35 47 812,-54 96 1,88-138-947,1 1 0,0-1 0,2 2 1,1-1-1,0 1 0,1 0 0,1 0 0,1 0 0,1 1 1,0 28-1,2-47-175,0 0 1,1 1-1,-1-1 1,0 0-1,1 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,3 1-1,37 13-4699</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4234.47">2174 660 6771,'-1'2'13453,"5"2"-12398,492-32-345,-210 6-657,44-18-45,-221 24 115,-91 11 93,-14 3-172,0 1 1,1 0 0,0 0-1,-1 0 1,1 1 0,-1 0 0,10 0-1,-14 0-30,0-2-17,0 1-26</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5011.4">3859 605 7043,'0'0'6360,"-6"14"-2310,-2-14-3994,-13-4 420,21 3-536,-1 0-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 0 1,1-2-1,2 27-51,-3-22 136,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,10-12-302,25-21 235,-35 32 22,-1 1-1,1-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1 0 0,0-1 1,-1 1-1,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,-1 1 0,1-1 1,-1 1-1,1-1 1,-1 0-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1 0-1,1 0 0,6 24 69,-6-21-65,0 1 4,1 0 0,-1 0 0,-1 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 0 1,-1 0-1,1 0 0,-3 6 0,2-8-423,-1 1-1,1 0 0,-1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,0-1-1,1 1 0,-1-1 1,0 0-1,0 0 1,0-1-1,-8 3 1,-31 8-7925</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2451.75">2124 0 5298,'0'0'11283,"-19"12"-11014,10-6-231,-7 3 32,0 1-1,2 1 0,-1 0 0,1 1 1,1 0-1,0 1 0,-14 18 1,18-18 74,-35 47 812,-54 96 1,88-138-947,1 1 0,0-1 0,2 2 1,1-1-1,0 1 0,1 0 0,1 0 0,1 0 0,1 1 1,0 28-1,2-47-175,0 0 1,1 1-1,-1-1 1,0 0-1,1 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,3 1-1,37 13-4699</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4234.46">2174 660 6771,'-1'2'13453,"5"2"-12398,492-32-345,-210 6-657,44-18-45,-221 24 115,-91 11 93,-14 3-172,0 1 1,1 0 0,0 0-1,-1 0 1,1 1 0,-1 0 0,10 0-1,-14 0-30,0-2-17,0 1-26</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5011.39">3859 605 7043,'0'0'6360,"-6"14"-2310,-2-14-3994,-13-4 420,21 3-536,-1 0-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 0 1,1-2-1,2 27-51,-3-22 136,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,10-12-302,25-21 235,-35 32 22,-1 1-1,1-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1 0 0,0-1 1,-1 1-1,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,-1 1 0,1-1 1,-1 1-1,1-1 1,-1 0-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1 0-1,1 0 0,6 24 69,-6-21-65,0 1 4,1 0 0,-1 0 0,-1 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 0 1,-1 0-1,1 0 0,-3 6 0,2-8-423,-1 1-1,1 0 0,-1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,0-1-1,1 1 0,-1-1 1,0 0-1,0 0 1,0-1-1,-8 3 1,-31 8-7925</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -25068,7 +25067,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">115 32 13910,'0'0'5331,"-5"-5"-4811,2 3-474,1-1-1,-1 1 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,-5-2 1,8 3-30,-1 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,1 0 0,-1 1 0,0-1-1,1 1 1,-2 0 0,1 0-3,0 1-1,1-1 1,-1 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,1-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,0 0-1,0-1 1,0 3 0,1 5 26,0 0 0,0 0 0,1 0 0,0 0 1,1-1-1,0 1 0,0-1 0,1 0 0,0 1 0,1-2 1,-1 1-1,10 11 0,20 37 172,-33-54-203,0-1 0,1 1 0,-1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1-1,-1-1 1,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,-4 2 0,-4 1-380,-1-1 0,1-1 0,-1 1 0,0-2 0,1 1 0,-1-2 0,-12 1 0,23-1 242,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 1,1-1-1,0 1 0,-1-1 0,1 1 0,0 0 1,0-1-1,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,1-1 1,-1 1-1,0 0 0,0-1 0,0 0 0,0 0-208,0-19-6054</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="256.97">55 73 7603,'0'0'9202,"14"-6"-8901,22-7 382,55-14 0,-75 25-360,-10 2-208,0-1-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1-1 1,1 0 0,-1 0 0,0-1-1,8-4 1,-13 4-867</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="256.96">55 73 7603,'0'0'9202,"14"-6"-8901,22-7 382,55-14 0,-75 25-360,-10 2-208,0-1-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1-1 1,1 0 0,-1 0 0,0-1-1,8-4 1,-13 4-867</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -25214,13 +25213,13 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">3812 70 10069,'0'0'11928,"0"-10"-10874,0-50 1827,0 64-2764,-1 106 12,-5-1 0,-5-1-1,-45 197 1,51-285-98,4-11 6,-2 0 0,1 0 0,-1-1 0,-6 13 0,8-20 41,1-24-1778,0-24-4484,0 20-2497</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2294.55">1346 32 2305,'0'0'15810,"0"-10"-13862,-24 415 2097,18-328-3699,-1-32-224,6-43-89,1 1 0,-1 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,-2 3 0,3-4 322,0-2-306,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0-3 0,0 0 18,-6-65-232,2-95 1,5 140 119,1 1 0,1 0 0,1 0 0,1 0 0,2 1 0,0 0 0,1 0 0,11-22 0,-16 39 35,0 0 0,0 0 0,1 0 0,0 0-1,0 1 1,0-1 0,0 1 0,1 0 0,0 1 0,-1-1 0,2 1 0,-1 0-1,0 0 1,0 0 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 1 0,0 0 0,0 0-1,0 0 1,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,7 3 0,-10-2 2,0 1 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0 1 1,-1-1-1,0 0 0,1 1 1,-1-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 6-1,2 10-29,-1 1-1,0 32 0,-2-45 27,-1 0 1,0 1 0,0 0 0,0-1 0,-1 1-1,0-1 1,0 1 0,-1-1 0,0 0 0,0 0-1,-1 0 1,0-1 0,0 1 0,-1-1 0,1 0-1,-1 0 1,-9 8 0,-2-1-30,0 1-1,0-2 0,-1 0 1,-37 18-1,33-24-71,2-1-73,19-5 165,0 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,0-1 1,0 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 1 1,-1-1 0,0 0-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 1 1,38 30 174,1-1 0,1-1 0,1-3 0,74 36 1,-112-61-757,8 3 1886</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2294.56">1346 32 2305,'0'0'15810,"0"-10"-13862,-24 415 2097,18-328-3699,-1-32-224,6-43-89,1 1 0,-1 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,-2 3 0,3-4 322,0-2-306,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0-3 0,0 0 18,-6-65-232,2-95 1,5 140 119,1 1 0,1 0 0,1 0 0,1 0 0,2 1 0,0 0 0,1 0 0,11-22 0,-16 39 35,0 0 0,0 0 0,1 0 0,0 0-1,0 1 1,0-1 0,0 1 0,1 0 0,0 1 0,-1-1 0,2 1 0,-1 0-1,0 0 1,0 0 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 1 0,0 0 0,0 0-1,0 0 1,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,7 3 0,-10-2 2,0 1 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0 1 1,-1-1-1,0 0 0,1 1 1,-1-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 6-1,2 10-29,-1 1-1,0 32 0,-2-45 27,-1 0 1,0 1 0,0 0 0,0-1 0,-1 1-1,0-1 1,0 1 0,-1-1 0,0 0 0,0 0-1,-1 0 1,0-1 0,0 1 0,-1-1 0,1 0-1,-1 0 1,-9 8 0,-2-1-30,0 1-1,0-2 0,-1 0 1,-37 18-1,33-24-71,2-1-73,19-5 165,0 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,0-1 1,0 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 1 1,-1-1 0,0 0-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 1 1,38 30 174,1-1 0,1-1 0,1-3 0,74 36 1,-112-61-757,8 3 1886</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1701.52">1815 187 11493,'0'0'10205,"1"-5"-9650,2 77 840,-2 66-205,-1-111-1046,0 36 176,-9 78 0,5-126 141,1-14-168,-5-26-70,-1-47-279,8 43-48,1-1 0,2 1 0,1 0 1,1-1-1,2 2 0,1-1 0,1 1 0,1 0 1,1 0-1,24-43 0,-30 65 98,-1 1 1,1 0-1,0 0 1,0 0-1,1 0 1,0 1-1,-1 0 1,1 0-1,1 0 1,-1 0-1,0 1 1,1 0-1,0 0 1,0 1-1,0-1 1,0 1-1,0 1 0,0-1 1,0 1-1,1 0 1,-1 0-1,0 1 1,1 0-1,-1 0 1,1 0-1,-1 1 1,7 1-1,-10 0 5,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-2 0 0,2 4 0,13 69 41,-8-20 118,-2 0 0,-2 1 1,-3-1-1,-3 0 0,-14 84 1,15-133 299,1-5-1465</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1483.4">1805 423 12966,'0'0'9012,"39"-19"-8804,0 13-112,10 1 144,-5-1-240,0 1 96,4-1-96,-9-2-1552,5 2-2834,-5-8-1905</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-729.33">2359 162 8404,'0'0'10954,"5"-9"-9428,-5 9-1519,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,11 87 1625,1 134-1,-11-213-1597,-2 0 0,1 0-1,-1 0 1,0 0 0,-1 0 0,1 0-1,-2 0 1,1-1 0,-1 1 0,0-1 0,-6 10-1,9-17-23,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,-3-12 212,2-17-137,1 29-76,0-24-55,0 0-1,2 0 1,0 0 0,2 0 0,1 0-1,1 0 1,1 1 0,1 0 0,1 1-1,1 0 1,1 0 0,1 1-1,24-34 1,-34 54 42,0-1-1,0 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 0,0-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0 1 0,1-1 0,-1 1 1,0-1-1,0 1 0,3 1 1,0 1 1,-1 0 0,0 0 1,1 0-1,-2 0 0,1 1 0,0 0 0,-1 0 1,1 0-1,-1 0 0,0 1 0,-1-1 1,1 1-1,-1 0 0,5 11 0,-2-2 15,-1 1 0,0-1 0,-1 2-1,-1-1 1,0 0 0,-1 0-1,-1 24 1,0-29 1,-2 1 0,1-1 0,-1 0 0,-1 0-1,0 0 1,0 0 0,-1 0 0,0 0 0,-1 0 0,0-1 0,-1 1 0,-7 10 0,11-17-19,0-3 3,1 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0-20 338,1 2-372,-1 7-3,1 1 0,0-1 0,0 0 0,1 0 0,1 1 0,0-1-1,0 1 1,1-1 0,0 1 0,1 0 0,5-10 0,2 0-149,1 0 0,1 1-1,1 1 1,1 0 0,33-32 0,-40 44 154,0-1 1,0 1-1,1 1 0,0 0 0,0 0 1,0 0-1,0 1 0,1 1 0,0-1 1,-1 2-1,1-1 0,0 2 0,1-1 1,-1 1-1,20 1 0,-27 0 35,0 0-1,0 1 1,0-1 0,-1 1-1,1 0 1,0-1 0,0 2-1,0-1 1,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 1-1,1 0 1,-1 0 0,0 0-1,3 3 1,-2 0 13,0 0-1,0-1 0,0 1 1,0 1-1,-1-1 0,0 0 1,0 1-1,2 8 1,-1 10 101,0 0 1,-1 0 0,-2 35-1,0-36 16,-1-6-55,-1 0-1,-1-1 1,0 1 0,-1-1 0,-1 1 0,-11 27 0,9-34-867,-2-8-6401</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8467.8">0 1000 4290,'0'0'17267,"21"-16"-15880,-13 12-1368,0 1 1,0 0-1,0 0 1,1 1-1,-1 0 1,1 1-1,0 0 1,-1 0-1,1 1 1,0 0-1,0 1 1,15 2-1,-23-2-23,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 0,1 0 1,-1 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,-1-1-1,1 1 0,0 0 1,-1-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0 0-1,0 0 0,-1 2 1,-1 53-147,1-48 144,0-1-21,0 0-1,-1 0 1,0-1 0,-1 1 0,1-1 0,-1 1 0,-1-1-1,0 0 1,0 0 0,0 0 0,-1 0 0,-8 8 0,3-4 56,-1 0 0,-1 0 0,0-1 0,0-1 0,-21 13 0,44-20 44,0-1-1,1 1 1,0-2-1,13 0 1,0 0-869,38 0-7418,-34-3-771</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9241.36">454 973 8148,'0'0'8358,"31"-11"-3945,-17 7-4295,0 0 0,1 1 1,-1 0-1,1 2 0,29-1 1,-43 10-122,1 0 1,-1 0 0,-1 0-1,1 0 1,-1 0 0,-1 0-1,-1 9 1,-3-4 6,-1 0 0,-1-1-1,0 1 1,0-1 0,-1-1 0,-1 1 0,0-1-1,-12 11 1,9-9 223,41-12-601,-21-2 340,0 0 0,0 1 0,0 0 0,0 1-1,11 1 1,-17 0 25,0 0 0,0 1-1,-1-1 1,1 0 0,-1 1 0,1-1-1,-1 1 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,0 0 0,0 0-1,0 0 1,-2 4 0,2-3 7,0 1-1,-1 0 1,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1-1,-1 0 1,0 0 0,-1 0 0,1 0 0,-4 3 0,-3 0 89,0 0 0,-1-2 0,0 1 0,0-1 1,-1 0-1,0-1 0,1 0 0,-1-1 0,0-1 0,-12 3 1,-36-1-3288,50-5-1552</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10024.45">912 1031 7876,'0'0'12453,"0"-6"-8251,0 8-4201,-1 12 24,1-1 1,1 1 0,0 0 0,1-1 0,6 23 0,-7-33-34,1 0-1,-1 0 0,0 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0-1 1,1 1-1,-1-1 0,1 0 1,0 0-1,-1 0 0,1 0 0,0-1 1,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1-1 0,0 1 1,1-1-1,6 0 0,-8 0-9,1-1 1,-1 1-1,0 0 0,1-1 0,-1 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,1 0 0,-1 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1-3 0,4-6 4,-2-1 0,0 0 0,5-21 0,0 0-8,-10 44-20,0 1-1,1-1 1,0 1-1,1 11 1,0 39 76,-9 43-943,3-54-3865,5-22 201</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8467.79">0 1000 4290,'0'0'17267,"21"-16"-15880,-13 12-1368,0 1 1,0 0-1,0 0 1,1 1-1,-1 0 1,1 1-1,0 0 1,-1 0-1,1 1 1,0 0-1,0 1 1,15 2-1,-23-2-23,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 0,1 0 1,-1 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,-1-1-1,1 1 0,0 0 1,-1-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0 0-1,0 0 0,-1 2 1,-1 53-147,1-48 144,0-1-21,0 0-1,-1 0 1,0-1 0,-1 1 0,1-1 0,-1 1 0,-1-1-1,0 0 1,0 0 0,0 0 0,-1 0 0,-8 8 0,3-4 56,-1 0 0,-1 0 0,0-1 0,0-1 0,-21 13 0,44-20 44,0-1-1,1 1 1,0-2-1,13 0 1,0 0-869,38 0-7418,-34-3-771</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9241.35">454 973 8148,'0'0'8358,"31"-11"-3945,-17 7-4295,0 0 0,1 1 1,-1 0-1,1 2 0,29-1 1,-43 10-122,1 0 1,-1 0 0,-1 0-1,1 0 1,-1 0 0,-1 0-1,-1 9 1,-3-4 6,-1 0 0,-1-1-1,0 1 1,0-1 0,-1-1 0,-1 1 0,0-1-1,-12 11 1,9-9 223,41-12-601,-21-2 340,0 0 0,0 1 0,0 0 0,0 1-1,11 1 1,-17 0 25,0 0 0,0 1-1,-1-1 1,1 0 0,-1 1 0,1-1-1,-1 1 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,0 0 0,0 0-1,0 0 1,-2 4 0,2-3 7,0 1-1,-1 0 1,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1-1,-1 0 1,0 0 0,-1 0 0,1 0 0,-4 3 0,-3 0 89,0 0 0,-1-2 0,0 1 0,0-1 1,-1 0-1,0-1 0,1 0 0,-1-1 0,0-1 0,-12 3 1,-36-1-3288,50-5-1552</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10024.44">912 1031 7876,'0'0'12453,"0"-6"-8251,0 8-4201,-1 12 24,1-1 1,1 1 0,0 0 0,1-1 0,6 23 0,-7-33-34,1 0-1,-1 0 0,0 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0-1 1,1 1-1,-1-1 0,1 0 1,0 0-1,-1 0 0,1 0 0,0-1 1,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1-1 0,0 1 1,1-1-1,6 0 0,-8 0-9,1-1 1,-1 1-1,0 0 0,1-1 0,-1 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,1 0 0,-1 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1-3 0,4-6 4,-2-1 0,0 0 0,5-21 0,0 0-8,-10 44-20,0 1-1,1-1 1,0 1-1,1 11 1,0 39 76,-9 43-943,3-54-3865,5-22 201</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10798.08">1498 944 5731,'0'0'9727,"-6"-2"-8631,-1 0-841,1 0 1,-1 1-1,0 0 0,0 0 0,0 0 1,-11 1-1,16 0-223,0 1 1,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 1 0,1-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1 0 0,0 0-1,-1 0 1,1 3-1,-1 7 19,0 0-1,1 1 0,1-1 1,0 1-1,0-1 1,1 0-1,1 1 1,0-1-1,1-1 0,0 1 1,1 0-1,0-1 1,8 12-1,-10-16-33,-1-2 73,14 33-126,-15-36 136,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,-1 0-1,0 3 1,-3-3-27,1 0 0,0 0-1,0-1 1,-1 0 0,1 1 0,-1-1 0,1 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,-4 0 0,-24-3-3168,30 1 2612,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,0 0 1,0-1-1,-1 1 1,1 0 0,1-1-1,-1 1 1,1-3-1,-1-2-1069,0-30-3256</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10938">1463 965 7828,'0'0'10660,"63"-50"-10483,-53 47-81,-1 3-96,1 0-32,0 0-1489,5 3-1168,-6 2-1617</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11736.71">1969 975 5138,'0'0'9890,"3"-6"-8372,0 0-847,4-7-306,-5-1 4930,-27 24-4783,16-3-484,0 1-1,1 1 1,0-1 0,1 1-1,-1 1 1,2-1-1,0 1 1,0 0-1,0 1 1,1-1-1,1 1 1,0 0 0,-3 14-1,2-5 5,1 0-1,1 0 0,1 0 1,0 1-1,2-1 1,3 37-1,-2-54-42,0-1-1,0 1 1,0 0 0,0-1-1,1 1 1,-1-1 0,1 0 0,-1 1-1,1-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,1 1 0,-1-1 0,0 1-1,1-1 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0-1 1,0 1 0,0-1-1,-1 0 1,6 0 0,-3 1-41,-1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,0-1 1,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1 0,6-6-1,-7 3 65,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,0-1-1,0 1 1,0-11-1,0 15-19,-1-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 1,1-1-1,0 1 0,-1 0 0,1 0 0,-3-1 0,-3 1-138,-1 0-1,1 1 1,0 0 0,0 0-1,0 0 1,-1 1-1,1 0 1,1 0 0,-1 1-1,-9 5 1,9-4-830,0 1 0,0 0 1,1 0-1,0 1 0,-9 10 1,0 3-4503</inkml:trace>
@@ -25261,9 +25260,9 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">50 61 4258,'0'0'10490,"0"13"-10578,-1 2 158,-1 1 1,-1-1-1,0 1 0,-8 22 1,5-19-12,1 0-1,-4 28 1,5-17-22,2-19 101,0 0 0,1 0 0,1 0-1,0 15 1,1-28-719,1-1 0,-1 0 0,1 1 0,-1-1 1,1 1-1,0 0 0,0 0 0,0 0 0,3-3 0,-1 1-1374,11-13-4546</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="620.85">294 73 6227,'0'0'6371,"5"-11"-5373,32 10-311,-18 0-534,0 1 0,26 3 1,-43-2-139,0-1-1,0 1 1,-1-1 0,1 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,-1 0 1,1 0 0,-1-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,0 2 0,0 1 41,1 1 0,-2-1 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-7 7 1,-63 58 303,71-69-342,5-1-51,0 0 29,-1 1-1,1-1 1,0 1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,0 1 0,1-1 0,-1 1-1,0 0 1,0 1 0,0-1 0,0 0-1,0 1 1,0 0 0,-1-1 0,1 1-1,-1 0 1,0 1 0,0-1 0,0 0 0,0 0-1,-1 1 1,1-1 0,-1 1 0,2 7-1,-4-10 30,1 0 0,-1 0-1,1 0 1,-1 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,1-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 1-1,0-1 1,-1 0-1,1 0 1,0 0 0,-1 0-1,-1 0 1,-53 0-46,43 0-198,13 0-139,-4 0 136</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1028.84">708 9 2865,'0'-3'13510,"-10"130"-11303,0 5-5841</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1466.68">821 1 2097,'0'0'9588,"5"8"-8593,-4 46 143,-2-47-1047,1 1-1,0 0 1,0-1-1,0 1 1,1 0 0,0-1-1,1 1 1,0 0 0,0-1-1,6 13 1,-7-18-77,0-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0 0 0,1 1-1,-1-1 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0-1 1,-1 1 0,1 0 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1 0,1-1-1,2 1 13,-1-1-1,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 1 0,1-1 1,-1 0-1,1 0 0,-1-1 1,3-3-1,36-64 927,-47 150-530,-7-5-151,-10 35-977,18-103-1637,-1-5-1626</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="620.84">294 73 6227,'0'0'6371,"5"-11"-5373,32 10-311,-18 0-534,0 1 0,26 3 1,-43-2-139,0-1-1,0 1 1,-1-1 0,1 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,-1 0 1,1 0 0,-1-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,0 2 0,0 1 41,1 1 0,-2-1 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-7 7 1,-63 58 303,71-69-342,5-1-51,0 0 29,-1 1-1,1-1 1,0 1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,0 1 0,1-1 0,-1 1-1,0 0 1,0 1 0,0-1 0,0 0-1,0 1 1,0 0 0,-1-1 0,1 1-1,-1 0 1,0 1 0,0-1 0,0 0 0,0 0-1,-1 1 1,1-1 0,-1 1 0,2 7-1,-4-10 30,1 0 0,-1 0-1,1 0 1,-1 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,1-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 1-1,0-1 1,-1 0-1,1 0 1,0 0 0,-1 0-1,-1 0 1,-53 0-46,43 0-198,13 0-139,-4 0 136</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1028.83">708 9 2865,'0'-3'13510,"-10"130"-11303,0 5-5841</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1466.67">821 1 2097,'0'0'9588,"5"8"-8593,-4 46 143,-2-47-1047,1 1-1,0 0 1,0-1-1,0 1 1,1 0 0,0-1-1,1 1 1,0 0 0,0-1-1,6 13 1,-7-18-77,0-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0 0 0,1 1-1,-1-1 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0-1 1,-1 1 0,1 0 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1 0,1-1-1,2 1 13,-1-1-1,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 1 0,1-1 1,-1 0-1,1 0 0,-1-1 1,3-3-1,36-64 927,-47 150-530,-7-5-151,-10 35-977,18-103-1637,-1-5-1626</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -25298,16 +25297,16 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2706.5">799 635 5731,'0'0'13851,"0"-16"-9982,-2 32-3762,0 0 0,-2 0 1,1 0-1,-12 27 0,2-1 128,-17 53 60,-12 49-3,41-143-291,1-1 0,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 0-1,0 0 1,1 1 0,-1-1 0,1 0 0,19 2 31,23-10-2,-19 3-227,-1-1-1,0-2 1,-1 0 0,0-1 0,39-23 0,-54 28 154,0-1 0,-1 1 0,0-1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,0-1 0,-1 0 0,0 0 0,1-13 0,-5 48 199,-1-1 0,-12 39 0,-9 47 96,17-41 210,1 94-1,7-164-600,10-22-7589,4-5-3141</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1891.79">1749 617 11045,'0'0'8524,"-16"-3"-7980,-55-7-141,67 10-353,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 1 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,-7 6 1,1 1 132,1 0 1,0 0 0,-13 17 0,7-8 96,4-5-205,0 1-1,1 0 1,0 0 0,1 1-1,1 0 1,1 1 0,0 0-1,0 0 1,2 0 0,0 1 0,1 0-1,1 0 1,0 0 0,2 0-1,0 31 1,1-44-66,0-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 1 0,0-1 1,0 0-1,0 0 0,1-1 0,-1 1 0,1 0 1,0 0-1,-1-1 0,1 1 0,1-1 0,-1 1 1,0-1-1,4 3 0,-1-2 27,-1 0 0,0-1-1,1 1 1,0-1 0,-1 0 0,1-1 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,10-1-1,-14 0 166,-1-1-198,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,0 0-1,1 0 1,-1 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 1 1,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,0 0-1,-1-1 1,1 1-4,0-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,-1 0 0,2 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1 0,1 0 0,-1-2 0,3 1-49,0 0 1,1 1-1,-1-1 0,1 0 0,-1 1 1,1 0-1,-1-1 0,1 1 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 1,6 1-1,-4-1-15,33-8-74,0 3 0,1 1 0,49 0 0,-86 5 148,0 1 1,-1 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1-1,-1 1 1,1 0-1,-1-1 1,0 1-1,0 0 1,0 3-1,5 50 578,-5-43-439,0 1 0,-1-1-1,0 0 1,-1 0 0,-1 0 0,-4 15-1,6-26-136,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,1-1 0,1 1-1,4 0-50,-1 0 0,1-1 0,0 1 0,-1-2-1,1 1 1,0-1 0,-1 0 0,10-3-1,-9 2-269,1-1-1,-1 0 1,0 0-1,0-1 1,0 0-1,0 0 1,-1-1-1,1 0 0,5-6 1,29-32-7437,-21 16 339</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1570.07">2142 761 9556,'0'0'11165,"1"-3"-10175,-1 3-917,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,0 31 373,-3 47-114,-2-37-114,-1-1 1,-14 47 0,0 3-41,19-83-499,0-7 241,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 1,-1-1-1,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-992.79">2157 731 2977,'0'0'18548,"2"-13"-17831,11-41-357,-11 51-341,1-1 0,-1 1-1,0 0 1,1 0 0,0 0 0,-1 1-1,1-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 1-1,1-1 1,-1 1 0,1 0-1,0-1 1,0 2 0,-1-1 0,7 0-1,1-2-2,20-3 60,0 1 1,1 1 0,58 2-1,-89 2-66,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,1 1 0,-1 0-1,0-1 1,1 1 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 3 0,0-1 13,-1 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 1 1,1-1-1,-2 6 0,0-1 39,0 1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,0 1 0,-7 13-1,-12 7-4,-1-1-1,-1-1 1,-1-1-1,-2-1 0,0-2 1,-41 28-1,68-51-61,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,1 1-1,26 3-182,46-4 20,-64-1 130,31-1-173,34-1-53,-69 3 250,0 0 0,0 0 0,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,6 3 0,-9-4 9,1 0 1,-1 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0 0-1,-1-1 1,1 1 0,0 0 0,-1-1-1,0 1 1,1 0 0,-1-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,-1 0 0,1-1 0,0 1-1,-1 0 1,0-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,-2 3 0,-2 2-12,-1 0 0,0 0 1,0 0-1,-1-1 0,1 0 0,-14 8 1,-2-2 100,1-1 1,-2 0 0,0-2 0,0-1 0,0-1-1,-32 5 1,1-4 22,-90-1 0,137-6-318,6 0 92,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-2 0,0 0 0,-5-21-6144</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-992.8">2157 731 2977,'0'0'18548,"2"-13"-17831,11-41-357,-11 51-341,1-1 0,-1 1-1,0 0 1,1 0 0,0 0 0,-1 1-1,1-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 1-1,1-1 1,-1 1 0,1 0-1,0-1 1,0 2 0,-1-1 0,7 0-1,1-2-2,20-3 60,0 1 1,1 1 0,58 2-1,-89 2-66,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,1 1 0,-1 0-1,0-1 1,1 1 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 3 0,0-1 13,-1 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 1 1,1-1-1,-2 6 0,0-1 39,0 1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,0 1 0,-7 13-1,-12 7-4,-1-1-1,-1-1 1,-1-1-1,-2-1 0,0-2 1,-41 28-1,68-51-61,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,1 1-1,26 3-182,46-4 20,-64-1 130,31-1-173,34-1-53,-69 3 250,0 0 0,0 0 0,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,6 3 0,-9-4 9,1 0 1,-1 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0 0-1,-1-1 1,1 1 0,0 0 0,-1-1-1,0 1 1,1 0 0,-1-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,-1 0 0,1-1 0,0 1-1,-1 0 1,0-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,-2 3 0,-2 2-12,-1 0 0,0 0 1,0 0-1,-1-1 0,1 0 0,-14 8 1,-2-2 100,1-1 1,-2 0 0,0-2 0,0-1 0,0-1-1,-32 5 1,1-4 22,-90-1 0,137-6-318,6 0 92,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-2 0,0 0 0,-5-21-6144</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63461.2">2778 165 1953,'0'0'9356,"1"-7"-8499,21-49 2541,-20 79-581,0 5-2695,0-1-1,-1 1 0,-2-1 0,-4 31 0,-3-22-693,6-12-6905</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63853.94">3036 84 4866,'0'0'7903,"-9"-2"-7130,-28-5-130,36 7-618,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1-1 1,-1 1-1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 2-1,-3 32 172,3-32-136,1 10 16,1-1-1,0 1 0,1-1 0,0 0 0,1 0 0,0 0 0,1 0 1,1-1-1,0 1 0,10 14 0,-15-26-86,-1 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,-1 1-1,1-1 1,0 0 0,0 1-1,0-1 1,0 1-1,-1-1 1,1 0-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1 0 1,0 0-1,1 0-229,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1 0 1,0-1-1,-1 1 0,1-1 0,0 1 0,-1-2 1,0-13-4642</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64041.52">3065 11 6259,'0'0'7827,"83"-11"-7362,-68 11-289,-11 0-160,6 0-32,-10 6-3090,0 5-1152</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64549.71">3328 68 4114,'0'0'8246,"0"-7"-7245,0-19-51,0 20 933,-1 12-1451,-19 75 366,13-61-664,1 0-1,1 1 0,2 0 1,-4 36-1,5-36 409,0-8-1902,2-3-3078</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65034.29">3531 62 4114,'0'0'7590,"0"-9"-5023,-1 35-1699,-2 0 1,-7 34 0,5-34-655,0 0-1,0 38 0,5-63-205,0 0-1,0 0 0,-1 1 0,1-1 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,34-1 177,-32 0-184,-3 0 4,0 0 1,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1-1 0,1-29 196,-1 22-94,-3 8-104,-1 0-1,0 0 1,1 1-1,-1-1 1,0 1-1,1 0 1,-1 0-1,-6 1 1,6-1-26,1 0-40,-1 1 0,0-1-1,1 1 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 1 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,-3 4 0,5-5-407,0 0 0,0 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,0-1 0,-1 1 1,1 1-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65034.28">3531 62 4114,'0'0'7590,"0"-9"-5023,-1 35-1699,-2 0 1,-7 34 0,5-34-655,0 0-1,0 38 0,5-63-205,0 0-1,0 0 0,-1 1 0,1-1 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,34-1 177,-32 0-184,-3 0 4,0 0 1,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1-1 0,1-29 196,-1 22-94,-3 8-104,-1 0-1,0 0 1,1 1-1,-1-1 1,0 1-1,1 0 1,-1 0-1,-6 1 1,6-1-26,1 0-40,-1 1 0,0-1-1,1 1 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 1 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,-3 4 0,5-5-407,0 0 0,0 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,0-1 0,-1 1 1,1 1-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65452.39">3921 138 3249,'0'0'6406,"0"-9"733,-2 41-6696,-1 0 0,-1-1 0,-2 0 0,-17 54 0,22-76-2949</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65764.4">3994 185 6659,'0'0'6841,"7"-1"-6615,102-1 324,-107 3-510,-1-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,-1 3 0,-1 46 1266,2-48-1265,-3 10 49,0-1-1,-1 1 1,-1-1-1,0 0 1,0 0 0,-1 0-1,0-1 1,-14 17-1,19-26-111,-8 7-5671</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="66201.51">4469 346 4578,'0'0'9604,"1"-5"-8299,0 3-1052,-1 0 0,0 0 0,1 0 0,-1 0-1,1 1 1,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,1 0 0,-1 1-1,1-2 1,-1 3 14,-1 18-344,-9 43 208,6-48-95,0 0 0,1 0 0,0 17 0,2-26 330,-1-3-506,1-1 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 1,0 1-1,0-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,17 1-5591</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="66852.41">4725 290 2225,'0'0'11819,"-24"9"-9624,20-6-2071,-1 1 0,1 0 0,0 0 0,1 0-1,-1 0 1,1 1 0,0-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,1 0 1,-1 1 0,1-1 0,0 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,1-1-1,1 9 1,-1-13-107,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,3 0-1,37 0 98,-33 0-87,-4 0-9,0 0 0,-1 0 0,1 0-1,0-1 1,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1-1 0,0 0 0,0 0-1,0 0 1,0 0 0,3-3-1,-3 1-8,0 0-1,0 0 0,0-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 1 1,-2-1-1,2-7 0,-1 8-9,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1-1,-1 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-3-4 0,-2 1 7,1-1 0,-2 1 1,1 0-1,0 1 0,-9-6 0,-12-10-11,22 18 11,1-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0 0,0-1-1,0 1 1,0-1-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,1-7 1,0 11-15,0-1-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 1,-1 0-1,1 0 1,2-1-1,53-1-122,-46 2 88,-8 0 31,1 0 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,0 1 0,-1 0-1,1 0 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0 0-1,0 0 1,5 4 0,-5-3-6,-1 1 1,0-1-1,0 1 1,0-1 0,0 1-1,-1 0 1,0 0-1,1 0 1,-1-1 0,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 1-1,-1 4 1,1 1 9,-1 1 1,0-1 0,-1 0-1,0 0 1,-1 0-1,0-1 1,0 1-1,-1 0 1,-1-1 0,1 0-1,-1 0 1,-1-1-1,-6 9 1,3-5-1269,-1-1 0,0-1 1,-1 0-1,0 0 0,-13 8 1,-10 3-9111</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65764.39">3994 185 6659,'0'0'6841,"7"-1"-6615,102-1 324,-107 3-510,-1-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,-1 3 0,-1 46 1266,2-48-1265,-3 10 49,0-1-1,-1 1 1,-1-1-1,0 0 1,0 0 0,-1 0-1,0-1 1,-14 17-1,19-26-111,-8 7-5671</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="66201.5">4469 346 4578,'0'0'9604,"1"-5"-8299,0 3-1052,-1 0 0,0 0 0,1 0 0,-1 0-1,1 1 1,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,1 0 0,-1 1-1,1-2 1,-1 3 14,-1 18-344,-9 43 208,6-48-95,0 0 0,1 0 0,0 17 0,2-26 330,-1-3-506,1-1 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 1,0 1-1,0-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,17 1-5591</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="66852.4">4725 290 2225,'0'0'11819,"-24"9"-9624,20-6-2071,-1 1 0,1 0 0,0 0 0,1 0-1,-1 0 1,1 1 0,0-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,1 0 1,-1 1 0,1-1 0,0 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,1-1-1,1 9 1,-1-13-107,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,3 0-1,37 0 98,-33 0-87,-4 0-9,0 0 0,-1 0 0,1 0-1,0-1 1,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1-1 0,0 0 0,0 0-1,0 0 1,0 0 0,3-3-1,-3 1-8,0 0-1,0 0 0,0-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 1 1,-2-1-1,2-7 0,-1 8-9,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1-1,-1 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-3-4 0,-2 1 7,1-1 0,-2 1 1,1 0-1,0 1 0,-9-6 0,-12-10-11,22 18 11,1-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0 0,0-1-1,0 1 1,0-1-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,1-7 1,0 11-15,0-1-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 1,-1 0-1,1 0 1,2-1-1,53-1-122,-46 2 88,-8 0 31,1 0 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,0 1 0,-1 0-1,1 0 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0 0-1,0 0 1,5 4 0,-5-3-6,-1 1 1,0-1-1,0 1 1,0-1 0,0 1-1,-1 0 1,0 0-1,1 0 1,-1-1 0,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 1-1,-1 4 1,1 1 9,-1 1 1,0-1 0,-1 0-1,0 0 1,-1 0-1,0-1 1,0 1-1,-1 0 1,-1-1 0,1 0-1,-1 0 1,-1-1-1,-6 9 1,3-5-1269,-1-1 0,0-1 1,-1 0-1,0 0 0,-13 8 1,-10 3-9111</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -25421,7 +25420,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">159 207 10229,'0'0'4268,"12"-9"-4121,5 0-61,-11 5-32,0 0 1,1 0-1,-1 0 1,-1 0-1,1-1 1,0 0-1,-1 0 1,6-8-1,-9 8 69,0 1-1,0-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,0 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 1 1,-2-6 0,1-9 485,1 19-594,0 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,0 0 0,0 0 1,-1 0-1,1-1 0,0 1 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0-1 0,-17 27 527,7-1-508,0-1 1,1 1 0,2 1-1,1-1 1,-6 49 0,3 137 188,-32-208-59,18-2-144,10-1 99,22 1 433,38-1-603,79-11 0,-56-7-2902,-64 12-1656</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="422.23">4 73 5939,'0'0'12213,"-4"-24"-11845,26 18-143,6-2-65,11 0-128,11 0-32,-1 2-481,4 2-799,-7 0-1313,-14 0-3746</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="422.22">4 73 5939,'0'0'12213,"-4"-24"-11845,26 18-143,6-2-65,11 0-128,11 0-32,-1 2-481,4 2-799,-7 0-1313,-14 0-3746</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16555.24">89 706 10517,'0'0'9778,"4"-10"-7903,1 27-1617,-1 1-1,-1-1 1,0 1-1,-1 0 0,0 0 1,-4 36-1,2-26-138,29-26-557,-20-1 433,1-2 0,-1 1 0,0-1 0,0-1 0,0 0 0,0 0 0,0-1-1,0 0 1,0 0 0,8-6 0,-13 7-33,0-1 1,0 1-1,-1-1 0,0 0 0,1 0 0,-1-1 1,0 1-1,-1 0 0,1-1 0,0 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,-1-1 0,1 1 1,-1-10-1,0 14 48,-11 15-164,5-4 265,0-1 1,1 1-1,0 0 1,0 1-1,1-1 1,1 1-1,0 0 1,-3 22-1,2 9-1086,2 48 1,2-80 242,0-17-3831,3-5-5137</inkml:trace>
 </inkml:ink>
 </file>
@@ -25565,7 +25564,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 713 6435,'0'0'12571,"4"0"-12350,221 13 800,-83-3-734,992 9 434,-1015-19-679,626-17 59,-558 17-66,683-11 184,318-28-201,-579-13 68,-100 4-126,-7 41 108,155-12 45,-98 2 681,-410 18-670,101 20 47,6 0 1264,-57-21-1083,-199 0-355,-11 0-1002,0-1-447,0 0 0,0-1 0,0 0 0,-14-4 0,17 4-68,-25-7-5991</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1297.1">4372 84 4530,'0'0'7043,"3"-12"-6056,7-32 203,-8 33-187,-1 11-357,0 1-626,1 1 0,-1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 4-1,0-5 12,3 246 1342,-5-128-900,4-106-235,4-15-660,9-25-2354,-9 15 171,9-13-3107</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1297.09">4372 84 4530,'0'0'7043,"3"-12"-6056,7-32 203,-8 33-187,-1 11-357,0 1-626,1 1 0,-1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 4-1,0-5 12,3 246 1342,-5-128-900,4-106-235,4-15-660,9-25-2354,-9 15 171,9-13-3107</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2365.03">4541 175 4786,'0'0'7417,"-12"-3"-6022,128 14 539,618-27 401,-303 6-2217,-44 3-60,525-5 69,-681 12-65,-197 2-115,59 10 0,-58-6 823,61 2-1,-95-10-760,0 0 0,-1-1-1,1 1 1,0-1 0,-1 1 0,0-1 0,1 1 0,-1-1-1,0 1 1,0-1 0,-1 1 0,0-5 0,-8-35 34,5 27-87,0 1-1,2-1 1,-2-28 0,-17 218-513,-2-2 623,9-93-1797,8-53-2439</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3508.88">4532 874 2801,'0'0'10608,"-9"-11"-9941,-25-32-179,32 42-462,0-1 1,1 1-1,-1 0 0,0-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 2 0,0-1 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 0,0-1 1,-2 2-1,-2 0 31,1 1-1,0-1 1,1 1-1,-1 0 1,0 1 0,-7 6-1,7-3-12,-1-1 1,1 1-1,0 0 0,1 0 1,0 1-1,0-1 0,1 1 0,0 0 1,0 0-1,1 0 0,0 0 1,0 1-1,1-1 0,0 1 0,0-1 1,1 1-1,0-1 0,1 0 1,1 11-1,-1-17-30,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0-1,1-1 1,-1 1 0,4 0 0,-3-1 12,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 1,-1-1-1,1 1 0,5-5 0,2-7 77,-1 0 1,0-1-1,-1-1 1,0 1 0,-2-1-1,1-1 1,-2 1-1,0-1 1,4-23-1,-1 12 1311,-9 56-564,0 3-1001,-20 266 247,21-293-92,-1 1-1,0 0 1,0-1 0,-1 0-1,0 1 1,0-1-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0-1,-1-1 1,1 0 0,-1 1-1,0-1 1,-5 4-1,0-2 3,0 0 0,0-1-1,0 0 1,-1-1 0,0 0-1,0 0 1,-20 4 0,-35 7-1103,-85 10 1,46-18-3231</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6083.6">8430 41 6243,'0'0'8983,"-8"-3"-8148,-4-1-466,8 2-124,0 0 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,-8 1 1147,24-2-1319,0 1 0,0 0-1,0 1 1,21 2 0,3 0 25,160-5 94,-195 7-195,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,-1 7-1,1-3 0,-3 13 23,0 0 0,-1-1 0,-2 1 0,0-1 0,-1 0 0,-13 26 0,2 0 1,3 0 12,-1 2-2370,3-19-6589</inkml:trace>
@@ -25655,7 +25654,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">4 48 5523,'0'0'4225,"0"-9"-4225,0 12-2913,0-1 2241,0 2 528,0-2 32</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="345.08">4 181 2369,'0'0'5555,"-3"-4"-5555</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="635.81">4 168 11957,'10'-4'1111,"0"2"0,0-1-1,0 1 1,1 1-1,-1 0 1,14 0-1,42 2-4530,-21 0-6947</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="635.8">4 168 11957,'10'-4'1111,"0"2"0,0-1-1,0 1 1,1 1-1,-1 0 1,14 0-1,42 2-4530,-21 0-6947</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="838.8">67 215 5186,'0'0'9941,"-33"11"-9509,36-11-320,7 2-80,13-2 144,4 0-32,3 0-144,3 0-320,-3 0-1233,-4 0-3153,-6-9-1376</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1178.98">213 109 6435,'0'0'11229,"-8"-6"-10402,-23-20-269,23 20-259,17 27-1022,4-8 778,1-1 0,0-1 0,0 0 0,1-1 0,17 8 0,26 18 140,-58-36-185,1 1 0,0-1 0,0 0-1,-1 1 1,1-1 0,0 1 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1-1,0 0 1,1-1 0,-1 1 0,1 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,1 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,-1 0-1,1-1 1,0 1 0,0 0 0,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 1 0,0-1 0,-1 1-1,-52 23 806,37-17-813,-4 9-56</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1695.1">731 215 13398,'0'0'7958,"-3"-9"-7467,2 6-467,-11-35 586,11 35-517,0 1-1,1-1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 1-1,-1-1 0,2-4 1,0 5-84,0 1 1,0 0 0,0-1 0,0 1 0,0 0 0,1 0-1,-1 0 1,0 1 0,0-1 0,1 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,1 0 0,3 1 0,40 2-65,-43-2 53,0-1 1,0 1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 1 1,-1-1-1,1 1 0,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,-1 0 1,1 1-1,-1-1 1,1 1-1,-1-1 1,0 1-1,0 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,-1 4-1,1-1-1,-1 0 0,0 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,-1-1-1,1 0 1,-1 0 0,-5 6 0,-1-3 9,-1 0-1,1-1 1,-1 0 0,-14 6-1,-27 18 15,52-30-20,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,1-1 0,-1 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,19 3 16,-18-3-17,122 4-568,-82-5-2293,-1-1-3423,-18-1-1304</inkml:trace>
@@ -25691,7 +25690,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">117 90 8148,'0'0'9263,"-40"1"-3389,33 4-5879,1 0 0,0 1 0,-1 0 0,2 1 0,-1-1 0,1 1 0,0 0 0,0 1 0,-3 7 0,5-10 2,1-1 0,0 1-1,0 0 1,0 0-1,1 0 1,0 0 0,0 1-1,0-1 1,0 0 0,1 0-1,0 1 1,0-1-1,0 0 1,1 0 0,2 10-1,-2-13 2,1 1-1,0-1 0,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 0,0-1 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 0 1,0 0-1,2-1 0,0 2-36,0-1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,-1 0 0,1 0-1,0-1 1,-1 0 0,1 0 0,4-2 0,-3-4 15,0 1 1,0-1 0,-1 0-1,0-1 1,0 1-1,-1-1 1,0 0 0,-1 0-1,0 0 1,0 0 0,-1-1-1,0 1 1,-1-1-1,0 0 1,0 1 0,-1-1-1,0 0 1,-1 1 0,0-1-1,-4-16 1,4 25 23,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1-1 1,0 1-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,-1 1-1,1-1 1,0 1-1,0-1 0,0 1 1,-1-1-1,1 1 1,0 0-1,-1-1 0,1 1 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 1,-1 0-1,1 1 1,-2 0-1,1 0-13,-1 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,-2 5 0,-3 19-2640,8-7-4758</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="292.51">355 147 12102,'4'-7'7291,"6"-11"-6056,-5 3-852</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="852.37">561 79 3490,'0'0'11402,"0"-6"-10436,0 5-865,0-1 0,0 0 1,0 1-1,-1-1 0,1 1 1,0-1-1,-1 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1 0-1,-1-1 0,1 1 1,-1 1-1,0-1 0,1 0 0,-1 0 1,1 0-1,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,-1 1 0,1-1-97,1-1-1,0 0 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 1,0-1-1,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,1-1 0,-1 0 1,0 1-1,0-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,1 2 0,-1 1 0,1-1-1,0 1 1,0-1-1,0 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,0-1-1,0 1 1,4 3-1,2-2 32,39 26 1,-47-30-33,-1 0 0,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 0,-1-1 1,1 1-1,0 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 1,1 0-1,-1 0 1,0-1-1,1 1 0,-1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1-1 0,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0-1 1,-1 1-1,-5 3 32,-1 0 0,0 0-1,0-1 1,0 0 0,0-1 0,0 0-1,-1 0 1,-8 1 0,16-3-117,10-12-8763,-1 3 3771</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1161.6">568 43 10005,'0'0'8403,"-4"-8"-8307,21 6-15,10-2-65,6-1 16,3-1-32,4 0-385,-3 0-1616,-4 1-2785</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1161.59">568 43 10005,'0'0'8403,"-4"-8"-8307,21 6-15,10-2-65,6-1 16,3-1-32,4 0-385,-3 0-1616,-4 1-2785</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -25722,7 +25721,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">67 298 7379,'0'0'8532,"10"0"-8468,9 0 80,8 0-48,0 0 97,-1-2-193,1 0-177,-4 2-591,3-2-881,-6-2-1744,-3 0-2498</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-248.87">60 212 9204,'7'-2'12338,"26"-11"-12254,-16 9-355,-1 0 0,1 1 1,0 1-1,0 1 0,0 0 0,22 2 1,-8 0-3595,-29-1 3331,-2 0 400,0 0 0,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,2 4-3471,-2 3-792</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="557.15">236 93 5795,'0'0'8051,"-8"-4"-7152,-20-14 243,27 18-1107,1 0 0,0-1 0,0 1 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1 0,0 0 0,0 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 1-1,0-1 1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,0 1 0,5 21-201,-1-18 191,0 0 0,0 1 0,1-2-1,-1 1 1,1 0 0,0-1 0,0 0 0,0 0 0,0 0-1,7 2 1,58 20 137,-38-20-683,-23-4 306,-1 1 1,1 0-1,-1 0 0,1 0 1,8 5-1,-16-7 226,-1 32-150,0-27 155,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,-1-1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,-6 6 0,-41 42 472,41-45-681,1-1 0,0 1-1,0 0 1,0 1 0,1-1 0,1 1 0,-1 1-1,1-1 1,-7 16 0,11-15-3409</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1366.18">664 228 6563,'0'0'9893,"23"-18"-9643,-20 15-127,1-1 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,-2-8 0,2 6 1387,-9 44-1646,3-9 185,2 0 0,1 1 0,1-1 0,2 40 0,1-29-38,-6-36-44,1 0 0,-1-1 1,1 0-1,-1 0 0,0 0 0,0 0 0,-5-1 0,9 1 29,-17-1 3,-29 7 93,46-7-159,23 0-66,128-4-143,-50-4-6686,-73 5 1367</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1366.17">664 228 6563,'0'0'9893,"23"-18"-9643,-20 15-127,1-1 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,-2-8 0,2 6 1387,-9 44-1646,3-9 185,2 0 0,1 1 0,1-1 0,2 40 0,1-29-38,-6-36-44,1 0 0,-1-1 1,1 0-1,-1 0 0,0 0 0,0 0 0,-5-1 0,9 1 29,-17-1 3,-29 7 93,46-7-159,23 0-66,128-4-143,-50-4-6686,-73 5 1367</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3292.84">1287 256 8628,'0'0'8964,"-1"-6"-8505,0 5-422,1-1 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 0,-3-2 0,-1 1 38,1 0 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,-8 0 0,7 0-26,0 0 0,0 0 1,0 1-1,0 0 0,0 1 1,0-1-1,1 1 1,-1 1-1,-6 2 0,10-3-53,1-1 0,-1 1-1,1 0 1,-1 0-1,1-1 1,0 2 0,0-1-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 1-1,1-1 1,-1 1 0,1 0-1,0-1 1,0 1-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 3 0,1-5 9,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 1,0-1-1,-1 1 0,2-1 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0-1 1,0 1-1,2 0 0,31-2 134,-27 1-190,0 0 0,-1 0 0,1-1 0,-1 0 0,1 0 0,-1-1 1,0 0-1,0 0 0,0 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,2-9 1,1-9 30,0-1 0,-2 1 0,-1-1 0,-1 0 1,-1-37-1,-25 146 703,22-74-576,1 1 1,0-1-1,0 1 1,1-1-1,0 1 1,1 0-1,0-1 1,1 1-1,3 12 1,-3-20-94,-1 1 1,1 0 0,-1-1 0,1 1 0,1-1 0,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0-1 1,5 0 0,2 1 12,0 0 0,-1-2 0,1 1-1,0-1 1,-1-1 0,1 0 0,-1 0 0,1-1-1,18-8 1,-25 9-15,0 0-1,0-1 0,-1 0 1,1 1-1,0-1 0,-1-1 1,0 1-1,0 0 1,0-1-1,0 0 0,0 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,-1 0 1,1-1-1,-1 1 0,0-1 1,0 1-1,0-1 0,0 1 1,-1-1-1,0-8 0,0 12-12,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,0 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 1 0,0-1 0,0 0 1,0 1-1,0-1 0,-1 1 0,-3 0-5,1 1 0,-1 0 0,1 0 1,0 0-1,0 1 0,0-1 0,0 1 0,0 0 0,1 0 1,-1 0-1,-3 5 0,4-4-8,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0 1,0 1-1,0-1 0,1 0 0,-1 1 0,1-1 0,0 9 0,1-12 15,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,1-1-1,-1 1 0,0-1 0,0 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,2-1 1,32-2-622,-29-2 617,-1 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,0-1 0,0 1 0,1-11 547,-3 59-708,0-41 169,0 1 1,0 0-1,0-1 1,0 1-1,1-1 0,-1 1 1,0-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1-1-1,-1 1 0,1 0 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 1,1-1-1,1 0 1,3 0 9,1-1 0,-1 0 0,1 0 0,-1-1 1,0 0-1,0 0 0,0 0 0,0-1 0,9-7 1,-13 8 17,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0-1 1,0 1-1,-1-1 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 0 1,0 0-1,-1 0 0,0 0 1,1 0-1,-2-5 0,1 8 136,4 41-269,-2-38 107,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,3 0 0,-1 0-4,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1-1 0,0 1 0,9-3 0,-12 2-12,-1 0 1,1 0-1,-1-1 1,1 1 0,-1 0-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,-1 1-1,2-4 1,10-36 578,-5 20 137,1 58-539,8 68-163,-6-47 34,4 101 0,-15-152-33,1 0 0,-1 0 0,-1-1 0,0 1 0,1 0 0,-2-1 0,1 1 0,-1-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-12 6 0,5-3 10,0-1 1,-1 0-1,0 0 1,0-2-1,0 0 1,-1 0-1,1-1 0,-1 0 1,0-2-1,-16 1 1,28-2-10,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 0 0,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,0 0 1,-2-4-1,1 2-2,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,1 0-1,-1-1 1,1-5 0,2-2-54,0 1 0,0 0 0,1 0 0,0 0 0,0 0 0,1 1 0,11-16 0,6-1-1656,44-41 0,-2 12-4204,-13 12-3774</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13474.11">4 694 7668,'0'0'7411,"-4"-4"-7251,14 4-80,3 0 0,7 0 0,0 0-64,4 0-16,-5 0-1280,1 2-3123,-3-2-1391</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13722.34">27 741 6771,'0'0'3842,"3"17"-2722,7-13-271,3-2 47,7 0-560,-3 0 81,6-2-241,0 2-48,0-2 0,0 0-128,-6 0-1729,0 0-3313</inkml:trace>
@@ -26169,7 +26168,7 @@
       <c r="F2" s="9"/>
     </row>
     <row r="4" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>866</v>
       </c>
       <c r="C4" s="9"/>
@@ -26178,7 +26177,7 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="12"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -26497,7 +26496,7 @@
       </c>
       <c r="D2">
         <f ca="1">RAND()</f>
-        <v>0.38724526286788563</v>
+        <v>0.14039843257991502</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -26506,7 +26505,7 @@
       </c>
       <c r="D4">
         <f ca="1">RANDBETWEEN(10,150)</f>
-        <v>147</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -26515,105 +26514,105 @@
       </c>
       <c r="D6" s="11" cm="1">
         <f t="array" aca="1" ref="D6:G8" ca="1">_xlfn.RANDARRAY(3,4,10,150,0)</f>
-        <v>133.25303448530019</v>
+        <v>95.392536672121651</v>
       </c>
       <c r="E6" s="11">
         <f ca="1"/>
-        <v>145.474203064904</v>
+        <v>18.775960479009171</v>
       </c>
       <c r="F6" s="11">
         <f ca="1"/>
-        <v>128.25074667354619</v>
+        <v>45.651342187897228</v>
       </c>
       <c r="G6" s="11">
         <f ca="1"/>
-        <v>132.80616224810214</v>
+        <v>140.474136495746</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="D7" s="11">
         <f ca="1"/>
-        <v>53.301300460361261</v>
+        <v>125.36848544180626</v>
       </c>
       <c r="E7" s="11">
         <f ca="1"/>
-        <v>136.39843553835593</v>
+        <v>47.961992539714714</v>
       </c>
       <c r="F7" s="11">
         <f ca="1"/>
-        <v>75.072490944632023</v>
+        <v>33.318021072645763</v>
       </c>
       <c r="G7" s="11">
         <f ca="1"/>
-        <v>83.086744636710819</v>
+        <v>132.42288300352766</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="D8" s="11">
         <f ca="1"/>
-        <v>95.046958806391984</v>
+        <v>119.12393237778358</v>
       </c>
       <c r="E8" s="11">
         <f ca="1"/>
-        <v>90.550746810904599</v>
+        <v>21.4491120848663</v>
       </c>
       <c r="F8" s="11">
         <f ca="1"/>
-        <v>36.184221738916449</v>
+        <v>87.738811594325171</v>
       </c>
       <c r="G8" s="11">
         <f ca="1"/>
-        <v>73.745400291658711</v>
+        <v>52.042517691772275</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="D10" cm="1">
         <f t="array" aca="1" ref="D10:E14" ca="1">_xlfn.RANDARRAY(5,2,150,500,1)</f>
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="E10">
         <f ca="1"/>
-        <v>479</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="D11">
         <f ca="1"/>
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E11">
         <f ca="1"/>
-        <v>204</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="D12">
         <f ca="1"/>
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="E12">
         <f ca="1"/>
-        <v>281</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="D13">
         <f ca="1"/>
-        <v>239</v>
+        <v>317</v>
       </c>
       <c r="E13">
         <f ca="1"/>
-        <v>448</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="D14">
         <f ca="1"/>
-        <v>304</v>
+        <v>237</v>
       </c>
       <c r="E14">
         <f ca="1"/>
-        <v>216</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -55771,7 +55770,7 @@
   <dimension ref="A2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B4" sqref="B4:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -56281,7 +56280,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">TODAY()</f>
-        <v>45837</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="3" spans="2:5">
@@ -56290,7 +56289,7 @@
       </c>
       <c r="C3" s="10">
         <f ca="1">NOW()</f>
-        <v>45837.903724884258</v>
+        <v>45879.830499189811</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -56308,15 +56307,15 @@
       </c>
       <c r="C5">
         <f ca="1">MONTH(C3)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" t="str">
         <f ca="1">TEXT(C3,"mmm")</f>
-        <v>Jun</v>
+        <v>Aug</v>
       </c>
       <c r="E5" t="str">
         <f ca="1">TEXT(C3,"mmmm")</f>
-        <v>June</v>
+        <v>August</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -56325,7 +56324,7 @@
       </c>
       <c r="C6">
         <f ca="1">WEEKNUM(C3)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -56343,7 +56342,7 @@
       </c>
       <c r="C8">
         <f ca="1">DAY(C3)</f>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D8" t="str">
         <f ca="1">TEXT(C3,"ddd")</f>
@@ -56360,7 +56359,7 @@
       </c>
       <c r="C9">
         <f ca="1">HOUR(C3)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -56369,7 +56368,7 @@
       </c>
       <c r="C10">
         <f ca="1">MINUTE(C3)</f>
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -56378,7 +56377,7 @@
       </c>
       <c r="C11">
         <f ca="1">SECOND(C3)</f>
-        <v>22</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -56387,7 +56386,7 @@
       </c>
       <c r="C12" s="2">
         <f ca="1">DATE(C4,C5,C8)</f>
-        <v>45837</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="13" spans="2:5">
@@ -56401,7 +56400,7 @@
       </c>
       <c r="C14" s="2">
         <f ca="1">EOMONTH(C3,2)</f>
-        <v>45900</v>
+        <v>45961</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -56414,11 +56413,11 @@
       </c>
       <c r="D15">
         <f ca="1">(C12-C13)/30</f>
-        <v>12.166666666666666</v>
+        <v>13.566666666666666</v>
       </c>
       <c r="E15">
         <f ca="1">C12-C13</f>
-        <v>365</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -56427,11 +56426,11 @@
       </c>
       <c r="C16">
         <f ca="1">YEARFRAC(C13,C12,1)</f>
-        <v>1</v>
+        <v>1.1135430916552667</v>
       </c>
     </row>
     <row r="21" spans="2:8">
-      <c r="C21" s="13">
+      <c r="C21" s="12">
         <v>45837.891050115744</v>
       </c>
       <c r="E21">
@@ -56440,7 +56439,7 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="C22" s="13">
+      <c r="C22" s="12">
         <v>45837.349386574075</v>
       </c>
     </row>
@@ -56453,19 +56452,19 @@
       </c>
       <c r="E29">
         <f ca="1">NETWORKDAYS(C29,TODAY(),C31:C33)</f>
-        <v>762</v>
-      </c>
-      <c r="F29" s="14">
+        <v>792</v>
+      </c>
+      <c r="F29">
         <f ca="1">TODAY()-C29</f>
-        <v>1067</v>
+        <v>1109</v>
       </c>
       <c r="G29">
         <f ca="1">NETWORKDAYS.INTL(C29,TODAY(),11,C31:C33)</f>
-        <v>912</v>
+        <v>948</v>
       </c>
       <c r="H29">
         <f ca="1">NETWORKDAYS.INTL(C29,TODAY(),13,C31:C33)</f>
-        <v>913</v>
+        <v>949</v>
       </c>
     </row>
     <row r="31" spans="2:8">

</xml_diff>